<commit_message>
Updated the code base
</commit_message>
<xml_diff>
--- a/InvoiceGenerator.TS/Helper/ExcelTemplates/TrueSouth/invoice-template.xlsx
+++ b/InvoiceGenerator.TS/Helper/ExcelTemplates/TrueSouth/invoice-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ebend\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Contracting\tdc-invoice-generator\InvoiceGenerator.TS\Helper\ExcelTemplates\TrueSouth\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3EBE35A-E485-4716-82C8-D0B88F20B9A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CBEF7EB-B78F-4C96-912D-2676C58E1F3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MasterSheet" sheetId="4" r:id="rId1"/>
@@ -68,6 +68,7 @@
         <sz val="16"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>FOOD SAFETY MANAGEMENT SYSTEM</t>
     </r>
@@ -77,6 +78,7 @@
         <sz val="18"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">
 </t>
@@ -87,6 +89,7 @@
         <sz val="18"/>
         <color rgb="FF5EBB47"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>DISPATCH PICKING SLIP</t>
     </r>
@@ -145,6 +148,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>STOCK INSPECTION CHEC</t>
     </r>
@@ -155,6 +159,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>K:</t>
     </r>
@@ -193,6 +198,7 @@
         <sz val="16"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>FOOD SAFETY MANAGEMENT SYSTEM</t>
     </r>
@@ -202,6 +208,7 @@
         <sz val="18"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">
 </t>
@@ -212,6 +219,7 @@
         <sz val="18"/>
         <color rgb="FF5EBB47"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>DISPATCH PICKING SLIP</t>
     </r>
@@ -221,6 +229,7 @@
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> (PAGE 2)</t>
     </r>
@@ -232,6 +241,7 @@
         <sz val="12"/>
         <color rgb="FF5EBB47"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">FOOD SAFETY MANAGEMENT SYSTEM
 </t>
@@ -242,6 +252,7 @@
         <sz val="16"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>Delivery Note</t>
     </r>
@@ -365,6 +376,7 @@
         <sz val="8"/>
         <color theme="0"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">Comply (Tick </t>
     </r>
@@ -383,6 +395,7 @@
         <sz val="8"/>
         <color theme="0"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> )</t>
     </r>
@@ -480,98 +493,116 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color rgb="FF5EBB47"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color rgb="FF5EBB47"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color theme="0"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="7"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color theme="0"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="8"/>
       <color theme="0"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -579,6 +610,7 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -586,6 +618,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -593,24 +626,28 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="18"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="18"/>
       <color rgb="FF5EBB47"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -618,12 +655,14 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="16"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -1525,6 +1564,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="39" fillId="6" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1535,62 +1577,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="9" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="9" fillId="5" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1598,105 +1590,115 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="9" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="9" fillId="5" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="18" fillId="6" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1719,32 +1721,69 @@
     <xf numFmtId="0" fontId="30" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="6" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="6" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3604,7 +3643,7 @@
   </sheetPr>
   <dimension ref="A1:K999"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
@@ -3624,17 +3663,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="12" customHeight="1">
-      <c r="A1" s="59"/>
-      <c r="B1" s="60"/>
+      <c r="A1" s="93"/>
+      <c r="B1" s="94"/>
       <c r="C1" s="51"/>
-      <c r="D1" s="86" t="s">
+      <c r="D1" s="79" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="81"/>
-      <c r="F1" s="81"/>
-      <c r="G1" s="81"/>
-      <c r="H1" s="81"/>
-      <c r="I1" s="82"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="64"/>
+      <c r="I1" s="65"/>
       <c r="J1" s="1" t="s">
         <v>1</v>
       </c>
@@ -3643,14 +3682,14 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="12" customHeight="1">
-      <c r="A2" s="61"/>
-      <c r="B2" s="62"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="55"/>
+      <c r="A2" s="95"/>
+      <c r="B2" s="96"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="56"/>
       <c r="J2" s="1" t="s">
         <v>2</v>
       </c>
@@ -3659,14 +3698,14 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="12" customHeight="1">
-      <c r="A3" s="61"/>
-      <c r="B3" s="62"/>
-      <c r="D3" s="54"/>
-      <c r="E3" s="54"/>
-      <c r="F3" s="54"/>
-      <c r="G3" s="54"/>
-      <c r="H3" s="54"/>
-      <c r="I3" s="55"/>
+      <c r="A3" s="95"/>
+      <c r="B3" s="96"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="56"/>
       <c r="J3" s="1" t="s">
         <v>3</v>
       </c>
@@ -3675,14 +3714,14 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="12" customHeight="1">
-      <c r="A4" s="61"/>
-      <c r="B4" s="62"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="54"/>
-      <c r="F4" s="54"/>
-      <c r="G4" s="54"/>
-      <c r="H4" s="54"/>
-      <c r="I4" s="55"/>
+      <c r="A4" s="95"/>
+      <c r="B4" s="96"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
+      <c r="F4" s="55"/>
+      <c r="G4" s="55"/>
+      <c r="H4" s="55"/>
+      <c r="I4" s="56"/>
       <c r="J4" s="1" t="s">
         <v>4</v>
       </c>
@@ -3691,15 +3730,15 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="12" customHeight="1">
-      <c r="A5" s="63"/>
-      <c r="B5" s="64"/>
+      <c r="A5" s="97"/>
+      <c r="B5" s="98"/>
       <c r="C5" s="52"/>
-      <c r="D5" s="84"/>
-      <c r="E5" s="84"/>
-      <c r="F5" s="84"/>
-      <c r="G5" s="84"/>
-      <c r="H5" s="84"/>
-      <c r="I5" s="85"/>
+      <c r="D5" s="67"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="67"/>
+      <c r="G5" s="67"/>
+      <c r="H5" s="67"/>
+      <c r="I5" s="68"/>
       <c r="J5" s="1" t="s">
         <v>28</v>
       </c>
@@ -3721,27 +3760,27 @@
       <c r="K6" s="3"/>
     </row>
     <row r="7" spans="1:11" ht="12" customHeight="1">
-      <c r="A7" s="78" t="s">
+      <c r="A7" s="80" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="54"/>
+      <c r="B7" s="55"/>
       <c r="C7" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="87" t="s">
+      <c r="D7" s="81" t="s">
         <v>87</v>
       </c>
-      <c r="E7" s="54"/>
-      <c r="F7" s="54"/>
+      <c r="E7" s="55"/>
+      <c r="F7" s="55"/>
       <c r="G7" s="5" t="s">
         <v>32</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="I7" s="76"/>
-      <c r="J7" s="66"/>
-      <c r="K7" s="68"/>
+      <c r="I7" s="82"/>
+      <c r="J7" s="61"/>
+      <c r="K7" s="62"/>
     </row>
     <row r="8" spans="1:11" ht="1.5" customHeight="1">
       <c r="A8" s="6"/>
@@ -3757,27 +3796,27 @@
       <c r="K8" s="3"/>
     </row>
     <row r="9" spans="1:11" ht="12" customHeight="1">
-      <c r="A9" s="78" t="s">
+      <c r="A9" s="80" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="54"/>
+      <c r="B9" s="55"/>
       <c r="C9" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="78" t="s">
+      <c r="D9" s="80" t="s">
         <v>34</v>
       </c>
-      <c r="E9" s="54"/>
-      <c r="F9" s="54"/>
+      <c r="E9" s="55"/>
+      <c r="F9" s="55"/>
       <c r="G9" s="9" t="s">
         <v>35</v>
       </c>
       <c r="H9" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="I9" s="76"/>
-      <c r="J9" s="66"/>
-      <c r="K9" s="68"/>
+      <c r="I9" s="82"/>
+      <c r="J9" s="61"/>
+      <c r="K9" s="62"/>
     </row>
     <row r="10" spans="1:11" ht="1.5" customHeight="1">
       <c r="A10" s="6"/>
@@ -3793,61 +3832,61 @@
       <c r="K10" s="3"/>
     </row>
     <row r="11" spans="1:11" ht="12" customHeight="1">
-      <c r="A11" s="78" t="s">
+      <c r="A11" s="80" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="54"/>
+      <c r="B11" s="55"/>
       <c r="C11" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="78">
+      <c r="D11" s="80">
         <v>4700281175</v>
       </c>
-      <c r="E11" s="54"/>
-      <c r="F11" s="54"/>
+      <c r="E11" s="55"/>
+      <c r="F11" s="55"/>
       <c r="G11" s="9" t="s">
         <v>37</v>
       </c>
       <c r="H11" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="I11" s="76"/>
-      <c r="J11" s="66"/>
-      <c r="K11" s="68"/>
+      <c r="I11" s="82"/>
+      <c r="J11" s="61"/>
+      <c r="K11" s="62"/>
     </row>
     <row r="12" spans="1:11" ht="1.5" customHeight="1">
-      <c r="A12" s="71"/>
-      <c r="B12" s="54"/>
-      <c r="C12" s="54"/>
-      <c r="D12" s="54"/>
-      <c r="E12" s="54"/>
-      <c r="F12" s="54"/>
-      <c r="G12" s="54"/>
-      <c r="H12" s="54"/>
-      <c r="I12" s="54"/>
-      <c r="J12" s="54"/>
-      <c r="K12" s="54"/>
+      <c r="A12" s="85"/>
+      <c r="B12" s="55"/>
+      <c r="C12" s="55"/>
+      <c r="D12" s="55"/>
+      <c r="E12" s="55"/>
+      <c r="F12" s="55"/>
+      <c r="G12" s="55"/>
+      <c r="H12" s="55"/>
+      <c r="I12" s="55"/>
+      <c r="J12" s="55"/>
+      <c r="K12" s="55"/>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13" s="77" t="s">
+      <c r="A13" s="91" t="s">
         <v>38</v>
       </c>
-      <c r="B13" s="54"/>
+      <c r="B13" s="55"/>
       <c r="C13" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="76"/>
-      <c r="E13" s="66"/>
-      <c r="F13" s="68"/>
+      <c r="D13" s="82"/>
+      <c r="E13" s="61"/>
+      <c r="F13" s="62"/>
       <c r="G13" s="11" t="s">
         <v>39</v>
       </c>
       <c r="H13" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="I13" s="76"/>
-      <c r="J13" s="66"/>
-      <c r="K13" s="68"/>
+      <c r="I13" s="82"/>
+      <c r="J13" s="61"/>
+      <c r="K13" s="62"/>
     </row>
     <row r="14" spans="1:11" ht="1.5" customHeight="1">
       <c r="A14" s="3"/>
@@ -3863,25 +3902,25 @@
       <c r="K14" s="3"/>
     </row>
     <row r="15" spans="1:11">
-      <c r="A15" s="78" t="s">
+      <c r="A15" s="80" t="s">
         <v>40</v>
       </c>
-      <c r="B15" s="54"/>
+      <c r="B15" s="55"/>
       <c r="C15" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="76"/>
-      <c r="E15" s="66"/>
-      <c r="F15" s="68"/>
+      <c r="D15" s="82"/>
+      <c r="E15" s="61"/>
+      <c r="F15" s="62"/>
       <c r="G15" s="9" t="s">
         <v>40</v>
       </c>
       <c r="H15" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="I15" s="76"/>
-      <c r="J15" s="66"/>
-      <c r="K15" s="68"/>
+      <c r="I15" s="82"/>
+      <c r="J15" s="61"/>
+      <c r="K15" s="62"/>
     </row>
     <row r="16" spans="1:11" ht="1.5" customHeight="1">
       <c r="A16" s="3"/>
@@ -3897,25 +3936,25 @@
       <c r="K16" s="3"/>
     </row>
     <row r="17" spans="1:11">
-      <c r="A17" s="78" t="s">
+      <c r="A17" s="80" t="s">
         <v>41</v>
       </c>
-      <c r="B17" s="54"/>
+      <c r="B17" s="55"/>
       <c r="C17" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D17" s="76"/>
-      <c r="E17" s="66"/>
-      <c r="F17" s="68"/>
+      <c r="D17" s="82"/>
+      <c r="E17" s="61"/>
+      <c r="F17" s="62"/>
       <c r="G17" s="9" t="s">
         <v>41</v>
       </c>
       <c r="H17" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="I17" s="79"/>
-      <c r="J17" s="66"/>
-      <c r="K17" s="68"/>
+      <c r="I17" s="92"/>
+      <c r="J17" s="61"/>
+      <c r="K17" s="62"/>
     </row>
     <row r="18" spans="1:11" ht="1.5" customHeight="1">
       <c r="A18" s="3"/>
@@ -3931,38 +3970,38 @@
       <c r="K18" s="3"/>
     </row>
     <row r="19" spans="1:11">
-      <c r="A19" s="78" t="s">
+      <c r="A19" s="80" t="s">
         <v>42</v>
       </c>
-      <c r="B19" s="54"/>
+      <c r="B19" s="55"/>
       <c r="C19" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D19" s="80"/>
-      <c r="E19" s="81"/>
-      <c r="F19" s="82"/>
+      <c r="D19" s="86"/>
+      <c r="E19" s="64"/>
+      <c r="F19" s="65"/>
       <c r="G19" s="9" t="s">
         <v>42</v>
       </c>
       <c r="H19" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="I19" s="80"/>
-      <c r="J19" s="81"/>
-      <c r="K19" s="82"/>
+      <c r="I19" s="86"/>
+      <c r="J19" s="64"/>
+      <c r="K19" s="65"/>
     </row>
     <row r="20" spans="1:11" ht="15.75" customHeight="1">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="8"/>
-      <c r="D20" s="83"/>
-      <c r="E20" s="84"/>
-      <c r="F20" s="85"/>
+      <c r="D20" s="66"/>
+      <c r="E20" s="67"/>
+      <c r="F20" s="68"/>
       <c r="G20" s="4"/>
       <c r="H20" s="3"/>
-      <c r="I20" s="83"/>
-      <c r="J20" s="84"/>
-      <c r="K20" s="85"/>
+      <c r="I20" s="66"/>
+      <c r="J20" s="67"/>
+      <c r="K20" s="68"/>
     </row>
     <row r="21" spans="1:11" ht="1.5" customHeight="1">
       <c r="A21" s="3"/>
@@ -3985,18 +4024,18 @@
       <c r="C22" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D22" s="76"/>
-      <c r="E22" s="66"/>
-      <c r="F22" s="68"/>
+      <c r="D22" s="82"/>
+      <c r="E22" s="61"/>
+      <c r="F22" s="62"/>
       <c r="G22" s="9" t="s">
         <v>44</v>
       </c>
       <c r="H22" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="I22" s="76"/>
-      <c r="J22" s="66"/>
-      <c r="K22" s="68"/>
+      <c r="I22" s="82"/>
+      <c r="J22" s="61"/>
+      <c r="K22" s="62"/>
     </row>
     <row r="23" spans="1:11" ht="1.5" customHeight="1">
       <c r="A23" s="3"/>
@@ -4012,57 +4051,57 @@
       <c r="K23" s="3"/>
     </row>
     <row r="24" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A24" s="78" t="s">
+      <c r="A24" s="80" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="54"/>
+      <c r="B24" s="55"/>
       <c r="C24" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D24" s="76"/>
-      <c r="E24" s="66"/>
-      <c r="F24" s="68"/>
+      <c r="D24" s="82"/>
+      <c r="E24" s="61"/>
+      <c r="F24" s="62"/>
       <c r="G24" s="9" t="s">
         <v>41</v>
       </c>
       <c r="H24" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="I24" s="76"/>
-      <c r="J24" s="66"/>
-      <c r="K24" s="68"/>
+      <c r="I24" s="82"/>
+      <c r="J24" s="61"/>
+      <c r="K24" s="62"/>
     </row>
     <row r="25" spans="1:11" ht="1.5" customHeight="1">
-      <c r="A25" s="71"/>
-      <c r="B25" s="54"/>
-      <c r="C25" s="54"/>
-      <c r="D25" s="54"/>
-      <c r="E25" s="54"/>
-      <c r="F25" s="54"/>
-      <c r="G25" s="54"/>
-      <c r="H25" s="54"/>
-      <c r="I25" s="54"/>
-      <c r="J25" s="54"/>
-      <c r="K25" s="54"/>
+      <c r="A25" s="85"/>
+      <c r="B25" s="55"/>
+      <c r="C25" s="55"/>
+      <c r="D25" s="55"/>
+      <c r="E25" s="55"/>
+      <c r="F25" s="55"/>
+      <c r="G25" s="55"/>
+      <c r="H25" s="55"/>
+      <c r="I25" s="55"/>
+      <c r="J25" s="55"/>
+      <c r="K25" s="55"/>
     </row>
     <row r="26" spans="1:11" ht="27" customHeight="1">
       <c r="A26" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="B26" s="75" t="s">
+      <c r="B26" s="90" t="s">
         <v>46</v>
       </c>
-      <c r="C26" s="74"/>
+      <c r="C26" s="89"/>
       <c r="D26" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="E26" s="72" t="s">
+      <c r="E26" s="87" t="s">
         <v>48</v>
       </c>
-      <c r="F26" s="73"/>
-      <c r="G26" s="73"/>
-      <c r="H26" s="73"/>
-      <c r="I26" s="74"/>
+      <c r="F26" s="88"/>
+      <c r="G26" s="88"/>
+      <c r="H26" s="88"/>
+      <c r="I26" s="89"/>
       <c r="J26" s="16" t="s">
         <v>49</v>
       </c>
@@ -4072,371 +4111,371 @@
     </row>
     <row r="27" spans="1:11" ht="12" customHeight="1">
       <c r="A27" s="17"/>
-      <c r="B27" s="69"/>
-      <c r="C27" s="55"/>
+      <c r="B27" s="70"/>
+      <c r="C27" s="56"/>
       <c r="D27" s="17"/>
-      <c r="E27" s="53"/>
-      <c r="F27" s="54"/>
-      <c r="G27" s="54"/>
-      <c r="H27" s="54"/>
-      <c r="I27" s="55"/>
+      <c r="E27" s="54"/>
+      <c r="F27" s="55"/>
+      <c r="G27" s="55"/>
+      <c r="H27" s="55"/>
+      <c r="I27" s="56"/>
       <c r="J27" s="20"/>
       <c r="K27" s="17"/>
     </row>
     <row r="28" spans="1:11" ht="12" customHeight="1">
       <c r="A28" s="18"/>
-      <c r="B28" s="70"/>
-      <c r="C28" s="58"/>
+      <c r="B28" s="71"/>
+      <c r="C28" s="59"/>
       <c r="D28" s="18"/>
-      <c r="E28" s="56"/>
-      <c r="F28" s="57"/>
-      <c r="G28" s="57"/>
-      <c r="H28" s="57"/>
-      <c r="I28" s="58"/>
+      <c r="E28" s="57"/>
+      <c r="F28" s="58"/>
+      <c r="G28" s="58"/>
+      <c r="H28" s="58"/>
+      <c r="I28" s="59"/>
       <c r="J28" s="19"/>
       <c r="K28" s="18"/>
     </row>
     <row r="29" spans="1:11" ht="12" customHeight="1">
       <c r="A29" s="17"/>
-      <c r="B29" s="69"/>
-      <c r="C29" s="55"/>
+      <c r="B29" s="70"/>
+      <c r="C29" s="56"/>
       <c r="D29" s="17"/>
-      <c r="E29" s="53"/>
-      <c r="F29" s="54"/>
-      <c r="G29" s="54"/>
-      <c r="H29" s="54"/>
-      <c r="I29" s="55"/>
+      <c r="E29" s="54"/>
+      <c r="F29" s="55"/>
+      <c r="G29" s="55"/>
+      <c r="H29" s="55"/>
+      <c r="I29" s="56"/>
       <c r="J29" s="20"/>
       <c r="K29" s="17"/>
     </row>
     <row r="30" spans="1:11" ht="12" customHeight="1">
       <c r="A30" s="18"/>
-      <c r="B30" s="70"/>
-      <c r="C30" s="58"/>
+      <c r="B30" s="71"/>
+      <c r="C30" s="59"/>
       <c r="D30" s="18"/>
-      <c r="E30" s="56"/>
-      <c r="F30" s="57"/>
-      <c r="G30" s="57"/>
-      <c r="H30" s="57"/>
-      <c r="I30" s="58"/>
+      <c r="E30" s="57"/>
+      <c r="F30" s="58"/>
+      <c r="G30" s="58"/>
+      <c r="H30" s="58"/>
+      <c r="I30" s="59"/>
       <c r="J30" s="19"/>
       <c r="K30" s="18"/>
     </row>
     <row r="31" spans="1:11" ht="12" customHeight="1">
       <c r="A31" s="17"/>
-      <c r="B31" s="69"/>
-      <c r="C31" s="55"/>
+      <c r="B31" s="70"/>
+      <c r="C31" s="56"/>
       <c r="D31" s="17"/>
-      <c r="E31" s="53"/>
-      <c r="F31" s="54"/>
-      <c r="G31" s="54"/>
-      <c r="H31" s="54"/>
-      <c r="I31" s="55"/>
+      <c r="E31" s="54"/>
+      <c r="F31" s="55"/>
+      <c r="G31" s="55"/>
+      <c r="H31" s="55"/>
+      <c r="I31" s="56"/>
       <c r="J31" s="20"/>
       <c r="K31" s="17"/>
     </row>
     <row r="32" spans="1:11" ht="12" customHeight="1">
       <c r="A32" s="18"/>
-      <c r="B32" s="70"/>
-      <c r="C32" s="58"/>
+      <c r="B32" s="71"/>
+      <c r="C32" s="59"/>
       <c r="D32" s="18"/>
-      <c r="E32" s="56"/>
-      <c r="F32" s="57"/>
-      <c r="G32" s="57"/>
-      <c r="H32" s="57"/>
-      <c r="I32" s="58"/>
+      <c r="E32" s="57"/>
+      <c r="F32" s="58"/>
+      <c r="G32" s="58"/>
+      <c r="H32" s="58"/>
+      <c r="I32" s="59"/>
       <c r="J32" s="19"/>
       <c r="K32" s="18"/>
     </row>
     <row r="33" spans="1:11" ht="12" customHeight="1">
       <c r="A33" s="17"/>
-      <c r="B33" s="69"/>
-      <c r="C33" s="55"/>
+      <c r="B33" s="70"/>
+      <c r="C33" s="56"/>
       <c r="D33" s="17"/>
-      <c r="E33" s="53"/>
-      <c r="F33" s="54"/>
-      <c r="G33" s="54"/>
-      <c r="H33" s="54"/>
-      <c r="I33" s="55"/>
+      <c r="E33" s="54"/>
+      <c r="F33" s="55"/>
+      <c r="G33" s="55"/>
+      <c r="H33" s="55"/>
+      <c r="I33" s="56"/>
       <c r="J33" s="20"/>
       <c r="K33" s="17"/>
     </row>
     <row r="34" spans="1:11" ht="12" customHeight="1">
       <c r="A34" s="18"/>
-      <c r="B34" s="70"/>
-      <c r="C34" s="58"/>
+      <c r="B34" s="71"/>
+      <c r="C34" s="59"/>
       <c r="D34" s="18"/>
-      <c r="E34" s="56"/>
-      <c r="F34" s="57"/>
-      <c r="G34" s="57"/>
-      <c r="H34" s="57"/>
-      <c r="I34" s="58"/>
+      <c r="E34" s="57"/>
+      <c r="F34" s="58"/>
+      <c r="G34" s="58"/>
+      <c r="H34" s="58"/>
+      <c r="I34" s="59"/>
       <c r="J34" s="19"/>
       <c r="K34" s="18"/>
     </row>
     <row r="35" spans="1:11" ht="12" customHeight="1">
       <c r="A35" s="17"/>
-      <c r="B35" s="69"/>
-      <c r="C35" s="55"/>
+      <c r="B35" s="70"/>
+      <c r="C35" s="56"/>
       <c r="D35" s="17"/>
-      <c r="E35" s="53"/>
-      <c r="F35" s="54"/>
-      <c r="G35" s="54"/>
-      <c r="H35" s="54"/>
-      <c r="I35" s="55"/>
+      <c r="E35" s="54"/>
+      <c r="F35" s="55"/>
+      <c r="G35" s="55"/>
+      <c r="H35" s="55"/>
+      <c r="I35" s="56"/>
       <c r="J35" s="20"/>
       <c r="K35" s="17"/>
     </row>
     <row r="36" spans="1:11" ht="12" customHeight="1">
       <c r="A36" s="18"/>
-      <c r="B36" s="70"/>
-      <c r="C36" s="58"/>
+      <c r="B36" s="71"/>
+      <c r="C36" s="59"/>
       <c r="D36" s="18"/>
-      <c r="E36" s="56"/>
-      <c r="F36" s="57"/>
-      <c r="G36" s="57"/>
-      <c r="H36" s="57"/>
-      <c r="I36" s="58"/>
+      <c r="E36" s="57"/>
+      <c r="F36" s="58"/>
+      <c r="G36" s="58"/>
+      <c r="H36" s="58"/>
+      <c r="I36" s="59"/>
       <c r="J36" s="19"/>
       <c r="K36" s="18"/>
     </row>
     <row r="37" spans="1:11" ht="12" customHeight="1">
       <c r="A37" s="17"/>
-      <c r="B37" s="69"/>
-      <c r="C37" s="55"/>
+      <c r="B37" s="70"/>
+      <c r="C37" s="56"/>
       <c r="D37" s="17"/>
-      <c r="E37" s="53"/>
-      <c r="F37" s="54"/>
-      <c r="G37" s="54"/>
-      <c r="H37" s="54"/>
-      <c r="I37" s="55"/>
+      <c r="E37" s="54"/>
+      <c r="F37" s="55"/>
+      <c r="G37" s="55"/>
+      <c r="H37" s="55"/>
+      <c r="I37" s="56"/>
       <c r="J37" s="20"/>
       <c r="K37" s="17"/>
     </row>
     <row r="38" spans="1:11" ht="12" customHeight="1">
       <c r="A38" s="18"/>
-      <c r="B38" s="70"/>
-      <c r="C38" s="58"/>
+      <c r="B38" s="71"/>
+      <c r="C38" s="59"/>
       <c r="D38" s="18"/>
-      <c r="E38" s="56"/>
-      <c r="F38" s="57"/>
-      <c r="G38" s="57"/>
-      <c r="H38" s="57"/>
-      <c r="I38" s="58"/>
+      <c r="E38" s="57"/>
+      <c r="F38" s="58"/>
+      <c r="G38" s="58"/>
+      <c r="H38" s="58"/>
+      <c r="I38" s="59"/>
       <c r="J38" s="19"/>
       <c r="K38" s="18"/>
     </row>
     <row r="39" spans="1:11" ht="12" customHeight="1">
       <c r="A39" s="17"/>
-      <c r="B39" s="69"/>
-      <c r="C39" s="55"/>
+      <c r="B39" s="70"/>
+      <c r="C39" s="56"/>
       <c r="D39" s="17"/>
-      <c r="E39" s="53"/>
-      <c r="F39" s="54"/>
-      <c r="G39" s="54"/>
-      <c r="H39" s="54"/>
-      <c r="I39" s="55"/>
+      <c r="E39" s="54"/>
+      <c r="F39" s="55"/>
+      <c r="G39" s="55"/>
+      <c r="H39" s="55"/>
+      <c r="I39" s="56"/>
       <c r="J39" s="20"/>
       <c r="K39" s="17"/>
     </row>
     <row r="40" spans="1:11" ht="12" customHeight="1">
       <c r="A40" s="18"/>
-      <c r="B40" s="70"/>
-      <c r="C40" s="58"/>
+      <c r="B40" s="71"/>
+      <c r="C40" s="59"/>
       <c r="D40" s="18"/>
-      <c r="E40" s="56"/>
-      <c r="F40" s="57"/>
-      <c r="G40" s="57"/>
-      <c r="H40" s="57"/>
-      <c r="I40" s="58"/>
+      <c r="E40" s="57"/>
+      <c r="F40" s="58"/>
+      <c r="G40" s="58"/>
+      <c r="H40" s="58"/>
+      <c r="I40" s="59"/>
       <c r="J40" s="19"/>
       <c r="K40" s="18"/>
     </row>
     <row r="41" spans="1:11" ht="12" customHeight="1">
       <c r="A41" s="17"/>
-      <c r="B41" s="69"/>
-      <c r="C41" s="55"/>
+      <c r="B41" s="70"/>
+      <c r="C41" s="56"/>
       <c r="D41" s="17"/>
-      <c r="E41" s="53"/>
-      <c r="F41" s="54"/>
-      <c r="G41" s="54"/>
-      <c r="H41" s="54"/>
-      <c r="I41" s="55"/>
+      <c r="E41" s="54"/>
+      <c r="F41" s="55"/>
+      <c r="G41" s="55"/>
+      <c r="H41" s="55"/>
+      <c r="I41" s="56"/>
       <c r="J41" s="20"/>
       <c r="K41" s="17"/>
     </row>
     <row r="42" spans="1:11" ht="12" customHeight="1">
       <c r="A42" s="18"/>
-      <c r="B42" s="70"/>
-      <c r="C42" s="58"/>
+      <c r="B42" s="71"/>
+      <c r="C42" s="59"/>
       <c r="D42" s="18"/>
-      <c r="E42" s="56"/>
-      <c r="F42" s="57"/>
-      <c r="G42" s="57"/>
-      <c r="H42" s="57"/>
-      <c r="I42" s="58"/>
+      <c r="E42" s="57"/>
+      <c r="F42" s="58"/>
+      <c r="G42" s="58"/>
+      <c r="H42" s="58"/>
+      <c r="I42" s="59"/>
       <c r="J42" s="19"/>
       <c r="K42" s="18"/>
     </row>
     <row r="43" spans="1:11" ht="12" customHeight="1">
       <c r="A43" s="17"/>
-      <c r="B43" s="69"/>
-      <c r="C43" s="55"/>
+      <c r="B43" s="70"/>
+      <c r="C43" s="56"/>
       <c r="D43" s="17"/>
-      <c r="E43" s="53"/>
-      <c r="F43" s="54"/>
-      <c r="G43" s="54"/>
-      <c r="H43" s="54"/>
-      <c r="I43" s="55"/>
+      <c r="E43" s="54"/>
+      <c r="F43" s="55"/>
+      <c r="G43" s="55"/>
+      <c r="H43" s="55"/>
+      <c r="I43" s="56"/>
       <c r="J43" s="20"/>
       <c r="K43" s="17"/>
     </row>
     <row r="44" spans="1:11" ht="12" customHeight="1">
       <c r="A44" s="18"/>
-      <c r="B44" s="70"/>
-      <c r="C44" s="58"/>
+      <c r="B44" s="71"/>
+      <c r="C44" s="59"/>
       <c r="D44" s="18"/>
-      <c r="E44" s="56"/>
-      <c r="F44" s="57"/>
-      <c r="G44" s="57"/>
-      <c r="H44" s="57"/>
-      <c r="I44" s="58"/>
+      <c r="E44" s="57"/>
+      <c r="F44" s="58"/>
+      <c r="G44" s="58"/>
+      <c r="H44" s="58"/>
+      <c r="I44" s="59"/>
       <c r="J44" s="19"/>
       <c r="K44" s="18"/>
     </row>
     <row r="45" spans="1:11" ht="1.5" customHeight="1">
-      <c r="A45" s="65"/>
-      <c r="B45" s="66"/>
-      <c r="C45" s="66"/>
-      <c r="D45" s="66"/>
-      <c r="E45" s="66"/>
-      <c r="F45" s="66"/>
-      <c r="G45" s="66"/>
-      <c r="H45" s="66"/>
-      <c r="I45" s="66"/>
-      <c r="J45" s="66"/>
-      <c r="K45" s="66"/>
+      <c r="A45" s="99"/>
+      <c r="B45" s="61"/>
+      <c r="C45" s="61"/>
+      <c r="D45" s="61"/>
+      <c r="E45" s="61"/>
+      <c r="F45" s="61"/>
+      <c r="G45" s="61"/>
+      <c r="H45" s="61"/>
+      <c r="I45" s="61"/>
+      <c r="J45" s="61"/>
+      <c r="K45" s="61"/>
     </row>
     <row r="46" spans="1:11" ht="15" customHeight="1">
-      <c r="A46" s="67" t="s">
+      <c r="A46" s="74" t="s">
         <v>51</v>
       </c>
-      <c r="B46" s="66"/>
-      <c r="C46" s="66"/>
-      <c r="D46" s="66"/>
-      <c r="E46" s="68"/>
-      <c r="F46" s="67" t="s">
+      <c r="B46" s="61"/>
+      <c r="C46" s="61"/>
+      <c r="D46" s="61"/>
+      <c r="E46" s="62"/>
+      <c r="F46" s="74" t="s">
         <v>52</v>
       </c>
-      <c r="G46" s="66"/>
-      <c r="H46" s="68"/>
-      <c r="I46" s="67" t="s">
+      <c r="G46" s="61"/>
+      <c r="H46" s="62"/>
+      <c r="I46" s="74" t="s">
         <v>53</v>
       </c>
-      <c r="J46" s="66"/>
-      <c r="K46" s="68"/>
+      <c r="J46" s="61"/>
+      <c r="K46" s="62"/>
     </row>
     <row r="47" spans="1:11" ht="18" customHeight="1">
-      <c r="A47" s="88" t="s">
+      <c r="A47" s="60" t="s">
         <v>54</v>
       </c>
-      <c r="B47" s="66"/>
-      <c r="C47" s="66"/>
-      <c r="D47" s="66"/>
-      <c r="E47" s="68"/>
-      <c r="F47" s="88" t="s">
+      <c r="B47" s="61"/>
+      <c r="C47" s="61"/>
+      <c r="D47" s="61"/>
+      <c r="E47" s="62"/>
+      <c r="F47" s="60" t="s">
         <v>55</v>
       </c>
-      <c r="G47" s="66"/>
-      <c r="H47" s="68"/>
-      <c r="I47" s="88" t="s">
+      <c r="G47" s="61"/>
+      <c r="H47" s="62"/>
+      <c r="I47" s="60" t="s">
         <v>55</v>
       </c>
-      <c r="J47" s="66"/>
-      <c r="K47" s="68"/>
+      <c r="J47" s="61"/>
+      <c r="K47" s="62"/>
     </row>
     <row r="48" spans="1:11" ht="17.25" customHeight="1">
-      <c r="A48" s="88" t="s">
+      <c r="A48" s="60" t="s">
         <v>56</v>
       </c>
-      <c r="B48" s="66"/>
-      <c r="C48" s="66"/>
-      <c r="D48" s="66"/>
-      <c r="E48" s="68"/>
-      <c r="F48" s="88" t="s">
+      <c r="B48" s="61"/>
+      <c r="C48" s="61"/>
+      <c r="D48" s="61"/>
+      <c r="E48" s="62"/>
+      <c r="F48" s="60" t="s">
         <v>57</v>
       </c>
-      <c r="G48" s="66"/>
-      <c r="H48" s="68"/>
-      <c r="I48" s="88" t="s">
+      <c r="G48" s="61"/>
+      <c r="H48" s="62"/>
+      <c r="I48" s="60" t="s">
         <v>57</v>
       </c>
-      <c r="J48" s="66"/>
-      <c r="K48" s="68"/>
+      <c r="J48" s="61"/>
+      <c r="K48" s="62"/>
     </row>
     <row r="49" spans="1:11" ht="17.25" customHeight="1">
-      <c r="A49" s="97" t="s">
+      <c r="A49" s="63" t="s">
         <v>58</v>
       </c>
-      <c r="B49" s="81"/>
-      <c r="C49" s="81"/>
-      <c r="D49" s="81"/>
-      <c r="E49" s="82"/>
-      <c r="F49" s="98" t="s">
+      <c r="B49" s="64"/>
+      <c r="C49" s="64"/>
+      <c r="D49" s="64"/>
+      <c r="E49" s="65"/>
+      <c r="F49" s="69" t="s">
         <v>59</v>
       </c>
-      <c r="G49" s="81"/>
-      <c r="H49" s="82"/>
-      <c r="I49" s="88" t="s">
+      <c r="G49" s="64"/>
+      <c r="H49" s="65"/>
+      <c r="I49" s="60" t="s">
         <v>60</v>
       </c>
-      <c r="J49" s="66"/>
-      <c r="K49" s="68"/>
+      <c r="J49" s="61"/>
+      <c r="K49" s="62"/>
     </row>
     <row r="50" spans="1:11" ht="27.6" customHeight="1">
-      <c r="A50" s="83"/>
-      <c r="B50" s="84"/>
-      <c r="C50" s="84"/>
-      <c r="D50" s="84"/>
-      <c r="E50" s="85"/>
-      <c r="F50" s="83"/>
-      <c r="G50" s="84"/>
-      <c r="H50" s="85"/>
-      <c r="I50" s="88" t="s">
+      <c r="A50" s="66"/>
+      <c r="B50" s="67"/>
+      <c r="C50" s="67"/>
+      <c r="D50" s="67"/>
+      <c r="E50" s="68"/>
+      <c r="F50" s="66"/>
+      <c r="G50" s="67"/>
+      <c r="H50" s="68"/>
+      <c r="I50" s="60" t="s">
         <v>61</v>
       </c>
-      <c r="J50" s="66"/>
-      <c r="K50" s="68"/>
+      <c r="J50" s="61"/>
+      <c r="K50" s="62"/>
     </row>
     <row r="51" spans="1:11" ht="1.5" customHeight="1">
-      <c r="A51" s="95" t="s">
+      <c r="A51" s="73" t="s">
         <v>62</v>
       </c>
-      <c r="B51" s="54"/>
-      <c r="C51" s="54"/>
-      <c r="D51" s="54"/>
-      <c r="E51" s="54"/>
-      <c r="F51" s="54"/>
-      <c r="G51" s="54"/>
-      <c r="H51" s="54"/>
-      <c r="I51" s="54"/>
-      <c r="J51" s="54"/>
-      <c r="K51" s="54"/>
+      <c r="B51" s="55"/>
+      <c r="C51" s="55"/>
+      <c r="D51" s="55"/>
+      <c r="E51" s="55"/>
+      <c r="F51" s="55"/>
+      <c r="G51" s="55"/>
+      <c r="H51" s="55"/>
+      <c r="I51" s="55"/>
+      <c r="J51" s="55"/>
+      <c r="K51" s="55"/>
     </row>
     <row r="52" spans="1:11" ht="15" customHeight="1">
-      <c r="A52" s="67" t="s">
+      <c r="A52" s="74" t="s">
         <v>63</v>
       </c>
-      <c r="B52" s="66"/>
-      <c r="C52" s="66"/>
-      <c r="D52" s="66"/>
-      <c r="E52" s="66"/>
-      <c r="F52" s="66"/>
-      <c r="G52" s="66"/>
-      <c r="H52" s="66"/>
-      <c r="I52" s="66"/>
-      <c r="J52" s="66"/>
-      <c r="K52" s="68"/>
+      <c r="B52" s="61"/>
+      <c r="C52" s="61"/>
+      <c r="D52" s="61"/>
+      <c r="E52" s="61"/>
+      <c r="F52" s="61"/>
+      <c r="G52" s="61"/>
+      <c r="H52" s="61"/>
+      <c r="I52" s="61"/>
+      <c r="J52" s="61"/>
+      <c r="K52" s="62"/>
     </row>
     <row r="53" spans="1:11" ht="13.5" customHeight="1">
       <c r="A53" s="21"/>
@@ -4445,137 +4484,137 @@
       <c r="D53" s="22"/>
       <c r="E53" s="22"/>
       <c r="F53" s="23"/>
-      <c r="G53" s="96" t="s">
+      <c r="G53" s="75" t="s">
         <v>64</v>
       </c>
-      <c r="H53" s="66"/>
-      <c r="I53" s="68"/>
-      <c r="J53" s="96" t="s">
+      <c r="H53" s="61"/>
+      <c r="I53" s="62"/>
+      <c r="J53" s="75" t="s">
         <v>65</v>
       </c>
-      <c r="K53" s="68"/>
+      <c r="K53" s="62"/>
     </row>
     <row r="54" spans="1:11" ht="12" customHeight="1">
-      <c r="A54" s="88" t="s">
+      <c r="A54" s="60" t="s">
         <v>66</v>
       </c>
-      <c r="B54" s="66"/>
-      <c r="C54" s="66"/>
-      <c r="D54" s="66"/>
-      <c r="E54" s="66"/>
-      <c r="F54" s="68"/>
-      <c r="G54" s="89"/>
-      <c r="H54" s="90"/>
-      <c r="I54" s="91"/>
-      <c r="J54" s="92"/>
-      <c r="K54" s="68"/>
+      <c r="B54" s="61"/>
+      <c r="C54" s="61"/>
+      <c r="D54" s="61"/>
+      <c r="E54" s="61"/>
+      <c r="F54" s="62"/>
+      <c r="G54" s="76"/>
+      <c r="H54" s="77"/>
+      <c r="I54" s="78"/>
+      <c r="J54" s="72"/>
+      <c r="K54" s="62"/>
     </row>
     <row r="55" spans="1:11" ht="12" customHeight="1">
-      <c r="A55" s="88" t="s">
+      <c r="A55" s="60" t="s">
         <v>67</v>
       </c>
-      <c r="B55" s="66"/>
-      <c r="C55" s="66"/>
-      <c r="D55" s="66"/>
-      <c r="E55" s="66"/>
-      <c r="F55" s="68"/>
-      <c r="G55" s="89"/>
-      <c r="H55" s="90"/>
-      <c r="I55" s="91"/>
-      <c r="J55" s="92"/>
-      <c r="K55" s="68"/>
+      <c r="B55" s="61"/>
+      <c r="C55" s="61"/>
+      <c r="D55" s="61"/>
+      <c r="E55" s="61"/>
+      <c r="F55" s="62"/>
+      <c r="G55" s="76"/>
+      <c r="H55" s="77"/>
+      <c r="I55" s="78"/>
+      <c r="J55" s="72"/>
+      <c r="K55" s="62"/>
     </row>
     <row r="56" spans="1:11" ht="12" customHeight="1">
-      <c r="A56" s="88" t="s">
+      <c r="A56" s="60" t="s">
         <v>68</v>
       </c>
-      <c r="B56" s="66"/>
-      <c r="C56" s="66"/>
-      <c r="D56" s="66"/>
-      <c r="E56" s="66"/>
-      <c r="F56" s="68"/>
-      <c r="G56" s="89"/>
-      <c r="H56" s="90"/>
-      <c r="I56" s="91"/>
-      <c r="J56" s="92"/>
-      <c r="K56" s="68"/>
+      <c r="B56" s="61"/>
+      <c r="C56" s="61"/>
+      <c r="D56" s="61"/>
+      <c r="E56" s="61"/>
+      <c r="F56" s="62"/>
+      <c r="G56" s="76"/>
+      <c r="H56" s="77"/>
+      <c r="I56" s="78"/>
+      <c r="J56" s="72"/>
+      <c r="K56" s="62"/>
     </row>
     <row r="57" spans="1:11" ht="12" customHeight="1">
-      <c r="A57" s="88" t="s">
+      <c r="A57" s="60" t="s">
         <v>69</v>
       </c>
-      <c r="B57" s="66"/>
-      <c r="C57" s="66"/>
-      <c r="D57" s="66"/>
-      <c r="E57" s="66"/>
-      <c r="F57" s="68"/>
-      <c r="G57" s="89"/>
-      <c r="H57" s="90"/>
-      <c r="I57" s="91"/>
-      <c r="J57" s="92"/>
-      <c r="K57" s="68"/>
+      <c r="B57" s="61"/>
+      <c r="C57" s="61"/>
+      <c r="D57" s="61"/>
+      <c r="E57" s="61"/>
+      <c r="F57" s="62"/>
+      <c r="G57" s="76"/>
+      <c r="H57" s="77"/>
+      <c r="I57" s="78"/>
+      <c r="J57" s="72"/>
+      <c r="K57" s="62"/>
     </row>
     <row r="58" spans="1:11" ht="12" customHeight="1">
-      <c r="A58" s="88" t="s">
+      <c r="A58" s="60" t="s">
         <v>70</v>
       </c>
-      <c r="B58" s="66"/>
-      <c r="C58" s="66"/>
-      <c r="D58" s="66"/>
-      <c r="E58" s="66"/>
-      <c r="F58" s="68"/>
-      <c r="G58" s="89"/>
-      <c r="H58" s="90"/>
-      <c r="I58" s="91"/>
-      <c r="J58" s="92"/>
-      <c r="K58" s="68"/>
+      <c r="B58" s="61"/>
+      <c r="C58" s="61"/>
+      <c r="D58" s="61"/>
+      <c r="E58" s="61"/>
+      <c r="F58" s="62"/>
+      <c r="G58" s="76"/>
+      <c r="H58" s="77"/>
+      <c r="I58" s="78"/>
+      <c r="J58" s="72"/>
+      <c r="K58" s="62"/>
     </row>
     <row r="59" spans="1:11" ht="12" customHeight="1">
-      <c r="A59" s="88" t="s">
+      <c r="A59" s="60" t="s">
         <v>71</v>
       </c>
-      <c r="B59" s="66"/>
-      <c r="C59" s="66"/>
-      <c r="D59" s="66"/>
-      <c r="E59" s="66"/>
-      <c r="F59" s="68"/>
-      <c r="G59" s="89"/>
-      <c r="H59" s="90"/>
-      <c r="I59" s="91"/>
-      <c r="J59" s="92"/>
-      <c r="K59" s="68"/>
+      <c r="B59" s="61"/>
+      <c r="C59" s="61"/>
+      <c r="D59" s="61"/>
+      <c r="E59" s="61"/>
+      <c r="F59" s="62"/>
+      <c r="G59" s="76"/>
+      <c r="H59" s="77"/>
+      <c r="I59" s="78"/>
+      <c r="J59" s="72"/>
+      <c r="K59" s="62"/>
     </row>
     <row r="60" spans="1:11" ht="12" customHeight="1">
-      <c r="A60" s="88" t="s">
+      <c r="A60" s="60" t="s">
         <v>72</v>
       </c>
-      <c r="B60" s="66"/>
-      <c r="C60" s="66"/>
-      <c r="D60" s="66"/>
-      <c r="E60" s="66"/>
-      <c r="F60" s="68"/>
-      <c r="G60" s="89"/>
-      <c r="H60" s="90"/>
-      <c r="I60" s="91"/>
-      <c r="J60" s="93" t="s">
+      <c r="B60" s="61"/>
+      <c r="C60" s="61"/>
+      <c r="D60" s="61"/>
+      <c r="E60" s="61"/>
+      <c r="F60" s="62"/>
+      <c r="G60" s="76"/>
+      <c r="H60" s="77"/>
+      <c r="I60" s="78"/>
+      <c r="J60" s="83" t="s">
         <v>86</v>
       </c>
-      <c r="K60" s="94"/>
+      <c r="K60" s="84"/>
     </row>
     <row r="61" spans="1:11" ht="12" customHeight="1">
-      <c r="A61" s="88" t="s">
+      <c r="A61" s="60" t="s">
         <v>73</v>
       </c>
-      <c r="B61" s="66"/>
-      <c r="C61" s="66"/>
-      <c r="D61" s="66"/>
-      <c r="E61" s="66"/>
-      <c r="F61" s="68"/>
-      <c r="G61" s="89"/>
-      <c r="H61" s="90"/>
-      <c r="I61" s="91"/>
-      <c r="J61" s="92"/>
-      <c r="K61" s="68"/>
+      <c r="B61" s="61"/>
+      <c r="C61" s="61"/>
+      <c r="D61" s="61"/>
+      <c r="E61" s="61"/>
+      <c r="F61" s="62"/>
+      <c r="G61" s="76"/>
+      <c r="H61" s="77"/>
+      <c r="I61" s="78"/>
+      <c r="J61" s="72"/>
+      <c r="K61" s="62"/>
     </row>
     <row r="62" spans="1:11" ht="15.75" customHeight="1"/>
     <row r="63" spans="1:11" ht="15.75" customHeight="1"/>
@@ -5517,37 +5556,61 @@
     <row r="999" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="110">
-    <mergeCell ref="E31:I31"/>
-    <mergeCell ref="E32:I32"/>
-    <mergeCell ref="E33:I33"/>
-    <mergeCell ref="A47:E47"/>
-    <mergeCell ref="F47:H47"/>
-    <mergeCell ref="I47:K47"/>
-    <mergeCell ref="A48:E48"/>
-    <mergeCell ref="F48:H48"/>
-    <mergeCell ref="A49:E50"/>
-    <mergeCell ref="F49:H50"/>
-    <mergeCell ref="I50:K50"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="E36:I36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="E35:I35"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="E34:I34"/>
-    <mergeCell ref="E38:I38"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="J56:K56"/>
-    <mergeCell ref="A51:K51"/>
-    <mergeCell ref="A52:K52"/>
-    <mergeCell ref="G53:I53"/>
-    <mergeCell ref="J53:K53"/>
-    <mergeCell ref="G54:I54"/>
-    <mergeCell ref="J54:K54"/>
-    <mergeCell ref="A54:F54"/>
-    <mergeCell ref="I48:K48"/>
-    <mergeCell ref="I49:K49"/>
+    <mergeCell ref="E29:I29"/>
+    <mergeCell ref="E30:I30"/>
+    <mergeCell ref="A1:B5"/>
+    <mergeCell ref="A45:K45"/>
+    <mergeCell ref="A46:E46"/>
+    <mergeCell ref="F46:H46"/>
+    <mergeCell ref="I46:K46"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="E43:I43"/>
+    <mergeCell ref="E44:I44"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="E39:I39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="E40:I40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="E41:I41"/>
+    <mergeCell ref="E42:I42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="E37:I37"/>
+    <mergeCell ref="A25:K25"/>
+    <mergeCell ref="E26:I26"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="I24:K24"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="I15:K15"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="I17:K17"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="D19:F20"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="E27:I27"/>
+    <mergeCell ref="E28:I28"/>
+    <mergeCell ref="A12:K12"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="I13:K13"/>
+    <mergeCell ref="I19:K20"/>
+    <mergeCell ref="I22:K22"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="I11:K11"/>
     <mergeCell ref="D1:I5"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="D7:F7"/>
@@ -5572,61 +5635,37 @@
     <mergeCell ref="J55:K55"/>
     <mergeCell ref="A56:F56"/>
     <mergeCell ref="G56:I56"/>
-    <mergeCell ref="A12:K12"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="I13:K13"/>
-    <mergeCell ref="I19:K20"/>
-    <mergeCell ref="I22:K22"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="I11:K11"/>
-    <mergeCell ref="A25:K25"/>
-    <mergeCell ref="E26:I26"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="I24:K24"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="I15:K15"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="I17:K17"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="D19:F20"/>
-    <mergeCell ref="D22:F22"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="E27:I27"/>
-    <mergeCell ref="E28:I28"/>
-    <mergeCell ref="E29:I29"/>
-    <mergeCell ref="E30:I30"/>
-    <mergeCell ref="A1:B5"/>
-    <mergeCell ref="A45:K45"/>
-    <mergeCell ref="A46:E46"/>
-    <mergeCell ref="F46:H46"/>
-    <mergeCell ref="I46:K46"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="E43:I43"/>
-    <mergeCell ref="E44:I44"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="E39:I39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="E40:I40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="E41:I41"/>
-    <mergeCell ref="E42:I42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="E37:I37"/>
+    <mergeCell ref="J56:K56"/>
+    <mergeCell ref="A51:K51"/>
+    <mergeCell ref="A52:K52"/>
+    <mergeCell ref="G53:I53"/>
+    <mergeCell ref="J53:K53"/>
+    <mergeCell ref="G54:I54"/>
+    <mergeCell ref="J54:K54"/>
+    <mergeCell ref="A54:F54"/>
+    <mergeCell ref="I48:K48"/>
+    <mergeCell ref="I49:K49"/>
+    <mergeCell ref="E31:I31"/>
+    <mergeCell ref="E32:I32"/>
+    <mergeCell ref="E33:I33"/>
+    <mergeCell ref="A47:E47"/>
+    <mergeCell ref="F47:H47"/>
+    <mergeCell ref="I47:K47"/>
+    <mergeCell ref="A48:E48"/>
+    <mergeCell ref="F48:H48"/>
+    <mergeCell ref="A49:E50"/>
+    <mergeCell ref="F49:H50"/>
+    <mergeCell ref="I50:K50"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="E36:I36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="E35:I35"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="E34:I34"/>
+    <mergeCell ref="E38:I38"/>
+    <mergeCell ref="B33:C33"/>
   </mergeCells>
   <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" sqref="J60:K60" xr:uid="{2AC316A1-1206-48C9-9C73-457461A6B233}">
@@ -6026,143 +6065,143 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A1" s="127"/>
-      <c r="B1" s="128"/>
-      <c r="C1" s="132" t="s">
+      <c r="A1" s="114"/>
+      <c r="B1" s="115"/>
+      <c r="C1" s="119" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="128"/>
-      <c r="E1" s="128"/>
-      <c r="F1" s="128"/>
-      <c r="G1" s="128"/>
-      <c r="H1" s="133"/>
+      <c r="D1" s="115"/>
+      <c r="E1" s="115"/>
+      <c r="F1" s="115"/>
+      <c r="G1" s="115"/>
+      <c r="H1" s="120"/>
       <c r="I1" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="136" t="s">
+      <c r="J1" s="123" t="s">
         <v>74</v>
       </c>
-      <c r="K1" s="137"/>
+      <c r="K1" s="124"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A2" s="129"/>
-      <c r="B2" s="54"/>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="134"/>
+      <c r="A2" s="116"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="121"/>
       <c r="I2" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="138" t="s">
+      <c r="J2" s="125" t="s">
         <v>78</v>
       </c>
-      <c r="K2" s="104"/>
+      <c r="K2" s="126"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A3" s="129"/>
-      <c r="B3" s="54"/>
-      <c r="C3" s="54"/>
-      <c r="D3" s="54"/>
-      <c r="E3" s="54"/>
-      <c r="F3" s="54"/>
-      <c r="G3" s="54"/>
-      <c r="H3" s="134"/>
+      <c r="A3" s="116"/>
+      <c r="B3" s="55"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="121"/>
       <c r="I3" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="138" t="s">
+      <c r="J3" s="125" t="s">
         <v>75</v>
       </c>
-      <c r="K3" s="104"/>
+      <c r="K3" s="126"/>
     </row>
     <row r="4" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A4" s="129"/>
-      <c r="B4" s="54"/>
-      <c r="C4" s="54"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="54"/>
-      <c r="F4" s="54"/>
-      <c r="G4" s="54"/>
-      <c r="H4" s="134"/>
+      <c r="A4" s="116"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
+      <c r="F4" s="55"/>
+      <c r="G4" s="55"/>
+      <c r="H4" s="121"/>
       <c r="I4" s="44" t="s">
         <v>76</v>
       </c>
-      <c r="J4" s="138" t="s">
+      <c r="J4" s="125" t="s">
         <v>77</v>
       </c>
-      <c r="K4" s="104"/>
+      <c r="K4" s="126"/>
     </row>
     <row r="5" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A5" s="130"/>
-      <c r="B5" s="131"/>
-      <c r="C5" s="131"/>
-      <c r="D5" s="131"/>
-      <c r="E5" s="131"/>
-      <c r="F5" s="131"/>
-      <c r="G5" s="131"/>
-      <c r="H5" s="135"/>
+      <c r="A5" s="117"/>
+      <c r="B5" s="118"/>
+      <c r="C5" s="118"/>
+      <c r="D5" s="118"/>
+      <c r="E5" s="118"/>
+      <c r="F5" s="118"/>
+      <c r="G5" s="118"/>
+      <c r="H5" s="122"/>
       <c r="I5" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="J5" s="139" t="s">
+      <c r="J5" s="127" t="s">
         <v>77</v>
       </c>
-      <c r="K5" s="140"/>
+      <c r="K5" s="128"/>
     </row>
     <row r="6" spans="1:11" ht="19.5" customHeight="1">
       <c r="A6" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="123" t="e" cm="1">
+      <c r="B6" s="134" t="e" cm="1">
         <f t="array" aca="1" ref="B6" ca="1">INDIRECT("Sheet1!"&amp;"D13")</f>
         <v>#REF!</v>
       </c>
-      <c r="C6" s="124"/>
-      <c r="D6" s="124"/>
-      <c r="E6" s="125"/>
-      <c r="F6" s="111" t="s">
+      <c r="C6" s="105"/>
+      <c r="D6" s="105"/>
+      <c r="E6" s="106"/>
+      <c r="F6" s="138" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="112"/>
-      <c r="H6" s="112"/>
-      <c r="I6" s="109" t="e" cm="1">
+      <c r="G6" s="139"/>
+      <c r="H6" s="139"/>
+      <c r="I6" s="136" t="e" cm="1">
         <f t="array" aca="1" ref="I6" ca="1">INDIRECT("Sheet1!"&amp;"I7")</f>
         <v>#REF!</v>
       </c>
-      <c r="J6" s="109"/>
-      <c r="K6" s="110"/>
+      <c r="J6" s="136"/>
+      <c r="K6" s="137"/>
     </row>
     <row r="7" spans="1:11" ht="19.5" customHeight="1">
       <c r="A7" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="126" t="e" cm="1">
+      <c r="B7" s="135" t="e" cm="1">
         <f t="array" aca="1" ref="B7" ca="1">INDIRECT("Sheet1!"&amp;"I11")</f>
         <v>#REF!</v>
       </c>
-      <c r="C7" s="106"/>
-      <c r="D7" s="106"/>
-      <c r="E7" s="107"/>
-      <c r="F7" s="115" t="s">
+      <c r="C7" s="101"/>
+      <c r="D7" s="101"/>
+      <c r="E7" s="102"/>
+      <c r="F7" s="142" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="116"/>
-      <c r="H7" s="116"/>
-      <c r="I7" s="113" t="e" cm="1">
+      <c r="G7" s="143"/>
+      <c r="H7" s="143"/>
+      <c r="I7" s="140" t="e" cm="1">
         <f t="array" aca="1" ref="I7" ca="1">INDIRECT("Sheet1!"&amp;"I9")</f>
         <v>#REF!</v>
       </c>
-      <c r="J7" s="113"/>
-      <c r="K7" s="114"/>
+      <c r="J7" s="140"/>
+      <c r="K7" s="141"/>
     </row>
     <row r="8" spans="1:11" ht="31.5">
-      <c r="A8" s="122" t="s">
+      <c r="A8" s="129" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="107"/>
+      <c r="B8" s="102"/>
       <c r="C8" s="27" t="s">
         <v>10</v>
       </c>
@@ -6172,14 +6211,14 @@
       <c r="E8" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="149" t="s">
+      <c r="F8" s="53" t="s">
         <v>88</v>
       </c>
-      <c r="G8" s="117" t="s">
+      <c r="G8" s="144" t="s">
         <v>13</v>
       </c>
-      <c r="H8" s="106"/>
-      <c r="I8" s="107"/>
+      <c r="H8" s="101"/>
+      <c r="I8" s="102"/>
       <c r="J8" s="27" t="s">
         <v>14</v>
       </c>
@@ -6188,11 +6227,11 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="27.4" customHeight="1">
-      <c r="A9" s="120" t="e" cm="1">
+      <c r="A9" s="130" t="e" cm="1">
         <f t="array" aca="1" ref="A9" ca="1">INDIRECT("Sheet1!"&amp;"E27")</f>
         <v>#REF!</v>
       </c>
-      <c r="B9" s="121"/>
+      <c r="B9" s="131"/>
       <c r="C9" s="29" t="e" cm="1">
         <f t="array" aca="1" ref="C9" ca="1">INDIRECT("Sheet1!"&amp;"A27")</f>
         <v>#REF!</v>
@@ -6206,18 +6245,18 @@
         <v>#REF!</v>
       </c>
       <c r="F9" s="32"/>
-      <c r="G9" s="108"/>
-      <c r="H9" s="106"/>
-      <c r="I9" s="107"/>
+      <c r="G9" s="100"/>
+      <c r="H9" s="101"/>
+      <c r="I9" s="102"/>
       <c r="J9" s="24"/>
       <c r="K9" s="33"/>
     </row>
     <row r="10" spans="1:11" ht="27.4" customHeight="1">
-      <c r="A10" s="118" t="e" cm="1">
+      <c r="A10" s="132" t="e" cm="1">
         <f t="array" aca="1" ref="A10" ca="1">INDIRECT("Sheet1!"&amp;"E28")</f>
         <v>#REF!</v>
       </c>
-      <c r="B10" s="119"/>
+      <c r="B10" s="133"/>
       <c r="C10" s="34" t="e" cm="1">
         <f t="array" aca="1" ref="C10" ca="1">INDIRECT("Sheet1!"&amp;"A28")</f>
         <v>#REF!</v>
@@ -6231,18 +6270,18 @@
         <v>#REF!</v>
       </c>
       <c r="F10" s="37"/>
-      <c r="G10" s="105"/>
-      <c r="H10" s="106"/>
-      <c r="I10" s="107"/>
+      <c r="G10" s="103"/>
+      <c r="H10" s="101"/>
+      <c r="I10" s="102"/>
       <c r="J10" s="38"/>
       <c r="K10" s="39"/>
     </row>
     <row r="11" spans="1:11" ht="27.4" customHeight="1">
-      <c r="A11" s="120" t="e" cm="1">
+      <c r="A11" s="130" t="e" cm="1">
         <f t="array" aca="1" ref="A11" ca="1">INDIRECT("Sheet1!"&amp;"E29")</f>
         <v>#REF!</v>
       </c>
-      <c r="B11" s="121"/>
+      <c r="B11" s="131"/>
       <c r="C11" s="29" t="e" cm="1">
         <f t="array" aca="1" ref="C11" ca="1">INDIRECT("Sheet1!"&amp;"A29")</f>
         <v>#REF!</v>
@@ -6256,18 +6295,18 @@
         <v>#REF!</v>
       </c>
       <c r="F11" s="32"/>
-      <c r="G11" s="108"/>
-      <c r="H11" s="106"/>
-      <c r="I11" s="107"/>
+      <c r="G11" s="100"/>
+      <c r="H11" s="101"/>
+      <c r="I11" s="102"/>
       <c r="J11" s="24"/>
       <c r="K11" s="33"/>
     </row>
     <row r="12" spans="1:11" ht="27.4" customHeight="1">
-      <c r="A12" s="118" t="e" cm="1">
+      <c r="A12" s="132" t="e" cm="1">
         <f t="array" aca="1" ref="A12" ca="1">INDIRECT("Sheet1!"&amp;"E30")</f>
         <v>#REF!</v>
       </c>
-      <c r="B12" s="119"/>
+      <c r="B12" s="133"/>
       <c r="C12" s="40" t="e" cm="1">
         <f t="array" aca="1" ref="C12" ca="1">INDIRECT("Sheet1!"&amp;"A30")</f>
         <v>#REF!</v>
@@ -6281,18 +6320,18 @@
         <v>#REF!</v>
       </c>
       <c r="F12" s="37"/>
-      <c r="G12" s="105"/>
-      <c r="H12" s="106"/>
-      <c r="I12" s="107"/>
+      <c r="G12" s="103"/>
+      <c r="H12" s="101"/>
+      <c r="I12" s="102"/>
       <c r="J12" s="38"/>
       <c r="K12" s="39"/>
     </row>
     <row r="13" spans="1:11" ht="27.4" customHeight="1">
-      <c r="A13" s="120" t="e" cm="1">
+      <c r="A13" s="130" t="e" cm="1">
         <f t="array" aca="1" ref="A13" ca="1">INDIRECT("Sheet1!"&amp;"E31")</f>
         <v>#REF!</v>
       </c>
-      <c r="B13" s="121"/>
+      <c r="B13" s="131"/>
       <c r="C13" s="41" t="e" cm="1">
         <f t="array" aca="1" ref="C13" ca="1">INDIRECT("Sheet1!"&amp;"A31")</f>
         <v>#REF!</v>
@@ -6306,18 +6345,18 @@
         <v>#REF!</v>
       </c>
       <c r="F13" s="32"/>
-      <c r="G13" s="108"/>
-      <c r="H13" s="106"/>
-      <c r="I13" s="107"/>
+      <c r="G13" s="100"/>
+      <c r="H13" s="101"/>
+      <c r="I13" s="102"/>
       <c r="J13" s="24"/>
       <c r="K13" s="33"/>
     </row>
     <row r="14" spans="1:11" ht="27.4" customHeight="1">
-      <c r="A14" s="118" t="e" cm="1">
+      <c r="A14" s="132" t="e" cm="1">
         <f t="array" aca="1" ref="A14" ca="1">INDIRECT("Sheet1!"&amp;"E32")</f>
         <v>#REF!</v>
       </c>
-      <c r="B14" s="119"/>
+      <c r="B14" s="133"/>
       <c r="C14" s="40" t="e" cm="1">
         <f t="array" aca="1" ref="C14" ca="1">INDIRECT("Sheet1!"&amp;"A32")</f>
         <v>#REF!</v>
@@ -6331,18 +6370,18 @@
         <v>#REF!</v>
       </c>
       <c r="F14" s="37"/>
-      <c r="G14" s="105"/>
-      <c r="H14" s="106"/>
-      <c r="I14" s="107"/>
+      <c r="G14" s="103"/>
+      <c r="H14" s="101"/>
+      <c r="I14" s="102"/>
       <c r="J14" s="38"/>
       <c r="K14" s="39"/>
     </row>
     <row r="15" spans="1:11" ht="27.4" customHeight="1">
-      <c r="A15" s="120" t="e" cm="1">
+      <c r="A15" s="130" t="e" cm="1">
         <f t="array" aca="1" ref="A15" ca="1">INDIRECT("Sheet1!"&amp;"E33")</f>
         <v>#REF!</v>
       </c>
-      <c r="B15" s="121"/>
+      <c r="B15" s="131"/>
       <c r="C15" s="41" t="e" cm="1">
         <f t="array" aca="1" ref="C15" ca="1">INDIRECT("Sheet1!"&amp;"A33")</f>
         <v>#REF!</v>
@@ -6356,18 +6395,18 @@
         <v>#REF!</v>
       </c>
       <c r="F15" s="32"/>
-      <c r="G15" s="108"/>
-      <c r="H15" s="106"/>
-      <c r="I15" s="107"/>
+      <c r="G15" s="100"/>
+      <c r="H15" s="101"/>
+      <c r="I15" s="102"/>
       <c r="J15" s="24"/>
       <c r="K15" s="33"/>
     </row>
     <row r="16" spans="1:11" ht="27.4" customHeight="1">
-      <c r="A16" s="118" t="e" cm="1">
+      <c r="A16" s="132" t="e" cm="1">
         <f t="array" aca="1" ref="A16" ca="1">INDIRECT("Sheet1!"&amp;"E34")</f>
         <v>#REF!</v>
       </c>
-      <c r="B16" s="119"/>
+      <c r="B16" s="133"/>
       <c r="C16" s="40" t="e" cm="1">
         <f t="array" aca="1" ref="C16" ca="1">INDIRECT("Sheet1!"&amp;"A34")</f>
         <v>#REF!</v>
@@ -6381,18 +6420,18 @@
         <v>#REF!</v>
       </c>
       <c r="F16" s="37"/>
-      <c r="G16" s="105"/>
-      <c r="H16" s="106"/>
-      <c r="I16" s="107"/>
+      <c r="G16" s="103"/>
+      <c r="H16" s="101"/>
+      <c r="I16" s="102"/>
       <c r="J16" s="38"/>
       <c r="K16" s="39"/>
     </row>
     <row r="17" spans="1:11" ht="27.4" customHeight="1">
-      <c r="A17" s="120" t="e" cm="1">
+      <c r="A17" s="130" t="e" cm="1">
         <f t="array" aca="1" ref="A17" ca="1">INDIRECT("Sheet1!"&amp;"E35")</f>
         <v>#REF!</v>
       </c>
-      <c r="B17" s="121"/>
+      <c r="B17" s="131"/>
       <c r="C17" s="41" t="e" cm="1">
         <f t="array" aca="1" ref="C17" ca="1">INDIRECT("Sheet1!"&amp;"A35")</f>
         <v>#REF!</v>
@@ -6406,18 +6445,18 @@
         <v>#REF!</v>
       </c>
       <c r="F17" s="32"/>
-      <c r="G17" s="108"/>
-      <c r="H17" s="106"/>
-      <c r="I17" s="107"/>
+      <c r="G17" s="100"/>
+      <c r="H17" s="101"/>
+      <c r="I17" s="102"/>
       <c r="J17" s="24"/>
       <c r="K17" s="33"/>
     </row>
     <row r="18" spans="1:11" ht="27.4" customHeight="1">
-      <c r="A18" s="118" t="e" cm="1">
+      <c r="A18" s="132" t="e" cm="1">
         <f t="array" aca="1" ref="A18" ca="1">INDIRECT("Sheet1!"&amp;"E36")</f>
         <v>#REF!</v>
       </c>
-      <c r="B18" s="119"/>
+      <c r="B18" s="133"/>
       <c r="C18" s="40" t="e" cm="1">
         <f t="array" aca="1" ref="C18" ca="1">INDIRECT("Sheet1!"&amp;"A36")</f>
         <v>#REF!</v>
@@ -6431,18 +6470,18 @@
         <v>#REF!</v>
       </c>
       <c r="F18" s="37"/>
-      <c r="G18" s="105"/>
-      <c r="H18" s="106"/>
-      <c r="I18" s="107"/>
+      <c r="G18" s="103"/>
+      <c r="H18" s="101"/>
+      <c r="I18" s="102"/>
       <c r="J18" s="38"/>
       <c r="K18" s="39"/>
     </row>
     <row r="19" spans="1:11" ht="27.4" customHeight="1">
-      <c r="A19" s="120" t="e" cm="1">
+      <c r="A19" s="130" t="e" cm="1">
         <f t="array" aca="1" ref="A19" ca="1">INDIRECT("Sheet1!"&amp;"E37")</f>
         <v>#REF!</v>
       </c>
-      <c r="B19" s="121"/>
+      <c r="B19" s="131"/>
       <c r="C19" s="41" t="e" cm="1">
         <f t="array" aca="1" ref="C19" ca="1">INDIRECT("Sheet1!"&amp;"A37")</f>
         <v>#REF!</v>
@@ -6456,18 +6495,18 @@
         <v>#REF!</v>
       </c>
       <c r="F19" s="32"/>
-      <c r="G19" s="108"/>
-      <c r="H19" s="106"/>
-      <c r="I19" s="107"/>
+      <c r="G19" s="100"/>
+      <c r="H19" s="101"/>
+      <c r="I19" s="102"/>
       <c r="J19" s="24"/>
       <c r="K19" s="33"/>
     </row>
     <row r="20" spans="1:11" ht="27.4" customHeight="1">
-      <c r="A20" s="118" t="e" cm="1">
+      <c r="A20" s="132" t="e" cm="1">
         <f t="array" aca="1" ref="A20" ca="1">INDIRECT("Sheet1!"&amp;"E38")</f>
         <v>#REF!</v>
       </c>
-      <c r="B20" s="119"/>
+      <c r="B20" s="133"/>
       <c r="C20" s="40" t="e" cm="1">
         <f t="array" aca="1" ref="C20" ca="1">INDIRECT("Sheet1!"&amp;"A38")</f>
         <v>#REF!</v>
@@ -6481,18 +6520,18 @@
         <v>#REF!</v>
       </c>
       <c r="F20" s="37"/>
-      <c r="G20" s="105"/>
-      <c r="H20" s="106"/>
-      <c r="I20" s="107"/>
+      <c r="G20" s="103"/>
+      <c r="H20" s="101"/>
+      <c r="I20" s="102"/>
       <c r="J20" s="38"/>
       <c r="K20" s="39"/>
     </row>
     <row r="21" spans="1:11" ht="27.4" customHeight="1">
-      <c r="A21" s="120" t="e" cm="1">
+      <c r="A21" s="130" t="e" cm="1">
         <f t="array" aca="1" ref="A21" ca="1">INDIRECT("Sheet1!"&amp;"E39")</f>
         <v>#REF!</v>
       </c>
-      <c r="B21" s="121"/>
+      <c r="B21" s="131"/>
       <c r="C21" s="41" t="e" cm="1">
         <f t="array" aca="1" ref="C21" ca="1">INDIRECT("Sheet1!"&amp;"A39")</f>
         <v>#REF!</v>
@@ -6506,18 +6545,18 @@
         <v>#REF!</v>
       </c>
       <c r="F21" s="32"/>
-      <c r="G21" s="108"/>
-      <c r="H21" s="106"/>
-      <c r="I21" s="107"/>
+      <c r="G21" s="100"/>
+      <c r="H21" s="101"/>
+      <c r="I21" s="102"/>
       <c r="J21" s="24"/>
       <c r="K21" s="33"/>
     </row>
     <row r="22" spans="1:11" ht="27.4" customHeight="1">
-      <c r="A22" s="118" t="e" cm="1">
+      <c r="A22" s="132" t="e" cm="1">
         <f t="array" aca="1" ref="A22" ca="1">INDIRECT("Sheet1!"&amp;"E40")</f>
         <v>#REF!</v>
       </c>
-      <c r="B22" s="119"/>
+      <c r="B22" s="133"/>
       <c r="C22" s="40" t="e" cm="1">
         <f t="array" aca="1" ref="C22" ca="1">INDIRECT("Sheet1!"&amp;"A40")</f>
         <v>#REF!</v>
@@ -6531,18 +6570,18 @@
         <v>#REF!</v>
       </c>
       <c r="F22" s="37"/>
-      <c r="G22" s="105"/>
-      <c r="H22" s="106"/>
-      <c r="I22" s="107"/>
+      <c r="G22" s="103"/>
+      <c r="H22" s="101"/>
+      <c r="I22" s="102"/>
       <c r="J22" s="38"/>
       <c r="K22" s="39"/>
     </row>
     <row r="23" spans="1:11" ht="27.4" customHeight="1">
-      <c r="A23" s="120" t="e" cm="1">
+      <c r="A23" s="130" t="e" cm="1">
         <f t="array" aca="1" ref="A23" ca="1">INDIRECT("Sheet1!"&amp;"E41")</f>
         <v>#REF!</v>
       </c>
-      <c r="B23" s="121"/>
+      <c r="B23" s="131"/>
       <c r="C23" s="41" t="e" cm="1">
         <f t="array" aca="1" ref="C23" ca="1">INDIRECT("Sheet1!"&amp;"A41")</f>
         <v>#REF!</v>
@@ -6556,18 +6595,18 @@
         <v>#REF!</v>
       </c>
       <c r="F23" s="32"/>
-      <c r="G23" s="108"/>
-      <c r="H23" s="106"/>
-      <c r="I23" s="107"/>
+      <c r="G23" s="100"/>
+      <c r="H23" s="101"/>
+      <c r="I23" s="102"/>
       <c r="J23" s="24"/>
       <c r="K23" s="33"/>
     </row>
     <row r="24" spans="1:11" ht="27.4" customHeight="1">
-      <c r="A24" s="118" t="e" cm="1">
+      <c r="A24" s="132" t="e" cm="1">
         <f t="array" aca="1" ref="A24" ca="1">INDIRECT("Sheet1!"&amp;"E42")</f>
         <v>#REF!</v>
       </c>
-      <c r="B24" s="119"/>
+      <c r="B24" s="133"/>
       <c r="C24" s="40" t="e" cm="1">
         <f t="array" aca="1" ref="C24" ca="1">INDIRECT("Sheet1!"&amp;"A42")</f>
         <v>#REF!</v>
@@ -6581,18 +6620,18 @@
         <v>#REF!</v>
       </c>
       <c r="F24" s="37"/>
-      <c r="G24" s="105"/>
-      <c r="H24" s="106"/>
-      <c r="I24" s="107"/>
+      <c r="G24" s="103"/>
+      <c r="H24" s="101"/>
+      <c r="I24" s="102"/>
       <c r="J24" s="38"/>
       <c r="K24" s="39"/>
     </row>
     <row r="25" spans="1:11" ht="27.4" customHeight="1">
-      <c r="A25" s="120" t="e" cm="1">
+      <c r="A25" s="130" t="e" cm="1">
         <f t="array" aca="1" ref="A25" ca="1">INDIRECT("Sheet1!"&amp;"E43")</f>
         <v>#REF!</v>
       </c>
-      <c r="B25" s="121"/>
+      <c r="B25" s="131"/>
       <c r="C25" s="41" t="e" cm="1">
         <f t="array" aca="1" ref="C25" ca="1">INDIRECT("Sheet1!"&amp;"A43")</f>
         <v>#REF!</v>
@@ -6606,18 +6645,18 @@
         <v>#REF!</v>
       </c>
       <c r="F25" s="32"/>
-      <c r="G25" s="108"/>
-      <c r="H25" s="106"/>
-      <c r="I25" s="107"/>
+      <c r="G25" s="100"/>
+      <c r="H25" s="101"/>
+      <c r="I25" s="102"/>
       <c r="J25" s="24"/>
       <c r="K25" s="33"/>
     </row>
     <row r="26" spans="1:11" ht="27.4" customHeight="1" thickBot="1">
-      <c r="A26" s="147" t="e" cm="1">
+      <c r="A26" s="107" t="e" cm="1">
         <f t="array" aca="1" ref="A26" ca="1">INDIRECT("Sheet1!"&amp;"E44")</f>
         <v>#REF!</v>
       </c>
-      <c r="B26" s="148"/>
+      <c r="B26" s="108"/>
       <c r="C26" s="40" t="e" cm="1">
         <f t="array" aca="1" ref="C26" ca="1">INDIRECT("Sheet1!"&amp;"A44")</f>
         <v>#REF!</v>
@@ -6631,177 +6670,177 @@
         <v>#REF!</v>
       </c>
       <c r="F26" s="37"/>
-      <c r="G26" s="105"/>
-      <c r="H26" s="106"/>
-      <c r="I26" s="107"/>
+      <c r="G26" s="103"/>
+      <c r="H26" s="101"/>
+      <c r="I26" s="102"/>
       <c r="J26" s="38"/>
       <c r="K26" s="39"/>
     </row>
     <row r="27" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A27" s="146" t="s">
+      <c r="A27" s="104" t="s">
         <v>16</v>
       </c>
-      <c r="B27" s="124"/>
-      <c r="C27" s="124"/>
-      <c r="D27" s="124"/>
-      <c r="E27" s="124"/>
-      <c r="F27" s="124"/>
-      <c r="G27" s="124"/>
-      <c r="H27" s="125"/>
+      <c r="B27" s="105"/>
+      <c r="C27" s="105"/>
+      <c r="D27" s="105"/>
+      <c r="E27" s="105"/>
+      <c r="F27" s="105"/>
+      <c r="G27" s="105"/>
+      <c r="H27" s="106"/>
       <c r="I27" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="J27" s="144" t="s">
+      <c r="J27" s="109" t="s">
         <v>18</v>
       </c>
-      <c r="K27" s="145"/>
+      <c r="K27" s="110"/>
     </row>
     <row r="28" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A28" s="141" t="s">
+      <c r="A28" s="113" t="s">
         <v>19</v>
       </c>
-      <c r="B28" s="106"/>
-      <c r="C28" s="106"/>
-      <c r="D28" s="106"/>
-      <c r="E28" s="106"/>
-      <c r="F28" s="106"/>
-      <c r="G28" s="106"/>
-      <c r="H28" s="107"/>
+      <c r="B28" s="101"/>
+      <c r="C28" s="101"/>
+      <c r="D28" s="101"/>
+      <c r="E28" s="101"/>
+      <c r="F28" s="101"/>
+      <c r="G28" s="101"/>
+      <c r="H28" s="102"/>
       <c r="I28" s="43"/>
-      <c r="J28" s="142"/>
-      <c r="K28" s="143"/>
+      <c r="J28" s="111"/>
+      <c r="K28" s="112"/>
     </row>
     <row r="29" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A29" s="141" t="s">
+      <c r="A29" s="113" t="s">
         <v>20</v>
       </c>
-      <c r="B29" s="106"/>
-      <c r="C29" s="106"/>
-      <c r="D29" s="106"/>
-      <c r="E29" s="106"/>
-      <c r="F29" s="106"/>
-      <c r="G29" s="106"/>
-      <c r="H29" s="107"/>
+      <c r="B29" s="101"/>
+      <c r="C29" s="101"/>
+      <c r="D29" s="101"/>
+      <c r="E29" s="101"/>
+      <c r="F29" s="101"/>
+      <c r="G29" s="101"/>
+      <c r="H29" s="102"/>
       <c r="I29" s="43"/>
-      <c r="J29" s="142"/>
-      <c r="K29" s="143"/>
+      <c r="J29" s="111"/>
+      <c r="K29" s="112"/>
     </row>
     <row r="30" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A30" s="141" t="s">
+      <c r="A30" s="113" t="s">
         <v>21</v>
       </c>
-      <c r="B30" s="106"/>
-      <c r="C30" s="106"/>
-      <c r="D30" s="106"/>
-      <c r="E30" s="106"/>
-      <c r="F30" s="106"/>
-      <c r="G30" s="106"/>
-      <c r="H30" s="107"/>
+      <c r="B30" s="101"/>
+      <c r="C30" s="101"/>
+      <c r="D30" s="101"/>
+      <c r="E30" s="101"/>
+      <c r="F30" s="101"/>
+      <c r="G30" s="101"/>
+      <c r="H30" s="102"/>
       <c r="I30" s="43"/>
-      <c r="J30" s="142"/>
-      <c r="K30" s="143"/>
+      <c r="J30" s="111"/>
+      <c r="K30" s="112"/>
     </row>
     <row r="31" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A31" s="141" t="s">
+      <c r="A31" s="113" t="s">
         <v>22</v>
       </c>
-      <c r="B31" s="106"/>
-      <c r="C31" s="106"/>
-      <c r="D31" s="106"/>
-      <c r="E31" s="106"/>
-      <c r="F31" s="106"/>
-      <c r="G31" s="106"/>
-      <c r="H31" s="107"/>
+      <c r="B31" s="101"/>
+      <c r="C31" s="101"/>
+      <c r="D31" s="101"/>
+      <c r="E31" s="101"/>
+      <c r="F31" s="101"/>
+      <c r="G31" s="101"/>
+      <c r="H31" s="102"/>
       <c r="I31" s="43"/>
-      <c r="J31" s="142"/>
-      <c r="K31" s="143"/>
+      <c r="J31" s="111"/>
+      <c r="K31" s="112"/>
     </row>
     <row r="32" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A32" s="141" t="s">
+      <c r="A32" s="113" t="s">
         <v>23</v>
       </c>
-      <c r="B32" s="106"/>
-      <c r="C32" s="106"/>
-      <c r="D32" s="106"/>
-      <c r="E32" s="106"/>
-      <c r="F32" s="106"/>
-      <c r="G32" s="106"/>
-      <c r="H32" s="107"/>
+      <c r="B32" s="101"/>
+      <c r="C32" s="101"/>
+      <c r="D32" s="101"/>
+      <c r="E32" s="101"/>
+      <c r="F32" s="101"/>
+      <c r="G32" s="101"/>
+      <c r="H32" s="102"/>
       <c r="I32" s="43"/>
-      <c r="J32" s="142"/>
-      <c r="K32" s="143"/>
+      <c r="J32" s="111"/>
+      <c r="K32" s="112"/>
     </row>
     <row r="33" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A33" s="141" t="s">
+      <c r="A33" s="113" t="s">
         <v>24</v>
       </c>
-      <c r="B33" s="106"/>
-      <c r="C33" s="106"/>
-      <c r="D33" s="106"/>
-      <c r="E33" s="106"/>
-      <c r="F33" s="106"/>
-      <c r="G33" s="106"/>
-      <c r="H33" s="107"/>
+      <c r="B33" s="101"/>
+      <c r="C33" s="101"/>
+      <c r="D33" s="101"/>
+      <c r="E33" s="101"/>
+      <c r="F33" s="101"/>
+      <c r="G33" s="101"/>
+      <c r="H33" s="102"/>
       <c r="I33" s="43"/>
-      <c r="J33" s="142"/>
-      <c r="K33" s="143"/>
+      <c r="J33" s="111"/>
+      <c r="K33" s="112"/>
     </row>
     <row r="34" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A34" s="141" t="s">
+      <c r="A34" s="113" t="s">
         <v>25</v>
       </c>
-      <c r="B34" s="106"/>
-      <c r="C34" s="106"/>
-      <c r="D34" s="106"/>
-      <c r="E34" s="106"/>
-      <c r="F34" s="106"/>
-      <c r="G34" s="106"/>
-      <c r="H34" s="107"/>
+      <c r="B34" s="101"/>
+      <c r="C34" s="101"/>
+      <c r="D34" s="101"/>
+      <c r="E34" s="101"/>
+      <c r="F34" s="101"/>
+      <c r="G34" s="101"/>
+      <c r="H34" s="102"/>
       <c r="I34" s="43"/>
-      <c r="J34" s="142"/>
-      <c r="K34" s="143"/>
+      <c r="J34" s="111"/>
+      <c r="K34" s="112"/>
     </row>
     <row r="35" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A35" s="100" t="s">
+      <c r="A35" s="146" t="s">
         <v>79</v>
       </c>
-      <c r="B35" s="101"/>
-      <c r="C35" s="101"/>
-      <c r="D35" s="101"/>
-      <c r="E35" s="101"/>
-      <c r="F35" s="101"/>
-      <c r="G35" s="101"/>
-      <c r="H35" s="102"/>
+      <c r="B35" s="147"/>
+      <c r="C35" s="147"/>
+      <c r="D35" s="147"/>
+      <c r="E35" s="147"/>
+      <c r="F35" s="147"/>
+      <c r="G35" s="147"/>
+      <c r="H35" s="148"/>
       <c r="I35" s="47"/>
-      <c r="J35" s="103"/>
-      <c r="K35" s="104"/>
+      <c r="J35" s="149"/>
+      <c r="K35" s="126"/>
     </row>
     <row r="36" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A36" s="99" t="s">
+      <c r="A36" s="145" t="s">
         <v>80</v>
       </c>
-      <c r="B36" s="99"/>
+      <c r="B36" s="145"/>
       <c r="C36" s="48"/>
     </row>
     <row r="37" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A37" s="99" t="s">
+      <c r="A37" s="145" t="s">
         <v>82</v>
       </c>
-      <c r="B37" s="99"/>
+      <c r="B37" s="145"/>
       <c r="C37" s="48"/>
     </row>
     <row r="38" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A38" s="99" t="s">
+      <c r="A38" s="145" t="s">
         <v>81</v>
       </c>
-      <c r="B38" s="99"/>
+      <c r="B38" s="145"/>
       <c r="C38" s="48"/>
     </row>
     <row r="39" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A39" s="99" t="s">
+      <c r="A39" s="145" t="s">
         <v>83</v>
       </c>
-      <c r="B39" s="99"/>
+      <c r="B39" s="145"/>
       <c r="C39" s="48"/>
     </row>
     <row r="40" spans="1:11" ht="15.75" customHeight="1"/>
@@ -7766,60 +7805,12 @@
     <row r="999" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="73">
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="G24:I24"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="G26:I26"/>
-    <mergeCell ref="A27:H27"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="J31:K31"/>
-    <mergeCell ref="J32:K32"/>
-    <mergeCell ref="A33:H33"/>
-    <mergeCell ref="J33:K33"/>
-    <mergeCell ref="A34:H34"/>
-    <mergeCell ref="J34:K34"/>
-    <mergeCell ref="A28:H28"/>
-    <mergeCell ref="A29:H29"/>
-    <mergeCell ref="J29:K29"/>
-    <mergeCell ref="A30:H30"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="A31:H31"/>
-    <mergeCell ref="A32:H32"/>
-    <mergeCell ref="A1:B5"/>
-    <mergeCell ref="C1:H5"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="G9:I9"/>
-    <mergeCell ref="G10:I10"/>
-    <mergeCell ref="G11:I11"/>
-    <mergeCell ref="G12:I12"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="G14:I14"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A35:H35"/>
+    <mergeCell ref="J35:K35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A38:B38"/>
     <mergeCell ref="G20:I20"/>
     <mergeCell ref="G21:I21"/>
     <mergeCell ref="G22:I22"/>
@@ -7833,12 +7824,60 @@
     <mergeCell ref="G18:I18"/>
     <mergeCell ref="G19:I19"/>
     <mergeCell ref="G8:I8"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A35:H35"/>
-    <mergeCell ref="J35:K35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="G10:I10"/>
+    <mergeCell ref="G11:I11"/>
+    <mergeCell ref="G12:I12"/>
+    <mergeCell ref="G13:I13"/>
+    <mergeCell ref="G14:I14"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="A1:B5"/>
+    <mergeCell ref="C1:H5"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="A34:H34"/>
+    <mergeCell ref="J34:K34"/>
+    <mergeCell ref="A28:H28"/>
+    <mergeCell ref="A29:H29"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="A30:H30"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="A31:H31"/>
+    <mergeCell ref="A32:H32"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="J31:K31"/>
+    <mergeCell ref="J32:K32"/>
+    <mergeCell ref="A33:H33"/>
+    <mergeCell ref="J33:K33"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="A27:H27"/>
+    <mergeCell ref="A26:B26"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.33" bottom="0.28000000000000003" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="62" fitToHeight="0" orientation="landscape" r:id="rId1"/>
@@ -7853,7 +7892,7 @@
   </sheetPr>
   <dimension ref="A1:K1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
@@ -7873,143 +7912,143 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A1" s="127"/>
-      <c r="B1" s="128"/>
-      <c r="C1" s="132" t="s">
+      <c r="A1" s="114"/>
+      <c r="B1" s="115"/>
+      <c r="C1" s="119" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="128"/>
-      <c r="E1" s="128"/>
-      <c r="F1" s="128"/>
-      <c r="G1" s="128"/>
-      <c r="H1" s="133"/>
+      <c r="D1" s="115"/>
+      <c r="E1" s="115"/>
+      <c r="F1" s="115"/>
+      <c r="G1" s="115"/>
+      <c r="H1" s="120"/>
       <c r="I1" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="136" t="s">
+      <c r="J1" s="123" t="s">
         <v>74</v>
       </c>
-      <c r="K1" s="137"/>
+      <c r="K1" s="124"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A2" s="129"/>
-      <c r="B2" s="54"/>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="134"/>
+      <c r="A2" s="116"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="121"/>
       <c r="I2" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="138" t="s">
+      <c r="J2" s="125" t="s">
         <v>78</v>
       </c>
-      <c r="K2" s="104"/>
+      <c r="K2" s="126"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A3" s="129"/>
-      <c r="B3" s="54"/>
-      <c r="C3" s="54"/>
-      <c r="D3" s="54"/>
-      <c r="E3" s="54"/>
-      <c r="F3" s="54"/>
-      <c r="G3" s="54"/>
-      <c r="H3" s="134"/>
+      <c r="A3" s="116"/>
+      <c r="B3" s="55"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="121"/>
       <c r="I3" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="138" t="s">
+      <c r="J3" s="125" t="s">
         <v>75</v>
       </c>
-      <c r="K3" s="104"/>
+      <c r="K3" s="126"/>
     </row>
     <row r="4" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A4" s="129"/>
-      <c r="B4" s="54"/>
-      <c r="C4" s="54"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="54"/>
-      <c r="F4" s="54"/>
-      <c r="G4" s="54"/>
-      <c r="H4" s="134"/>
+      <c r="A4" s="116"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
+      <c r="F4" s="55"/>
+      <c r="G4" s="55"/>
+      <c r="H4" s="121"/>
       <c r="I4" s="44" t="s">
         <v>76</v>
       </c>
-      <c r="J4" s="138" t="s">
+      <c r="J4" s="125" t="s">
         <v>77</v>
       </c>
-      <c r="K4" s="104"/>
+      <c r="K4" s="126"/>
     </row>
     <row r="5" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A5" s="130"/>
-      <c r="B5" s="131"/>
-      <c r="C5" s="131"/>
-      <c r="D5" s="131"/>
-      <c r="E5" s="131"/>
-      <c r="F5" s="131"/>
-      <c r="G5" s="131"/>
-      <c r="H5" s="135"/>
+      <c r="A5" s="117"/>
+      <c r="B5" s="118"/>
+      <c r="C5" s="118"/>
+      <c r="D5" s="118"/>
+      <c r="E5" s="118"/>
+      <c r="F5" s="118"/>
+      <c r="G5" s="118"/>
+      <c r="H5" s="122"/>
       <c r="I5" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="J5" s="139" t="s">
+      <c r="J5" s="127" t="s">
         <v>77</v>
       </c>
-      <c r="K5" s="140"/>
+      <c r="K5" s="128"/>
     </row>
     <row r="6" spans="1:11" ht="19.5" customHeight="1">
       <c r="A6" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="123" t="e" cm="1">
+      <c r="B6" s="134" t="e" cm="1">
         <f t="array" aca="1" ref="B6" ca="1">INDIRECT("Sheet1!"&amp;"D13")</f>
         <v>#REF!</v>
       </c>
-      <c r="C6" s="124"/>
-      <c r="D6" s="124"/>
-      <c r="E6" s="125"/>
-      <c r="F6" s="111" t="s">
+      <c r="C6" s="105"/>
+      <c r="D6" s="105"/>
+      <c r="E6" s="106"/>
+      <c r="F6" s="138" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="112"/>
-      <c r="H6" s="112"/>
-      <c r="I6" s="109" t="e" cm="1">
+      <c r="G6" s="139"/>
+      <c r="H6" s="139"/>
+      <c r="I6" s="136" t="e" cm="1">
         <f t="array" aca="1" ref="I6" ca="1">INDIRECT("Sheet1!"&amp;"I7")</f>
         <v>#REF!</v>
       </c>
-      <c r="J6" s="109"/>
-      <c r="K6" s="110"/>
+      <c r="J6" s="136"/>
+      <c r="K6" s="137"/>
     </row>
     <row r="7" spans="1:11" ht="19.5" customHeight="1">
       <c r="A7" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="126" t="e" cm="1">
+      <c r="B7" s="135" t="e" cm="1">
         <f t="array" aca="1" ref="B7" ca="1">INDIRECT("Sheet1!"&amp;"I11")</f>
         <v>#REF!</v>
       </c>
-      <c r="C7" s="106"/>
-      <c r="D7" s="106"/>
-      <c r="E7" s="107"/>
-      <c r="F7" s="115" t="s">
+      <c r="C7" s="101"/>
+      <c r="D7" s="101"/>
+      <c r="E7" s="102"/>
+      <c r="F7" s="142" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="116"/>
-      <c r="H7" s="116"/>
-      <c r="I7" s="113" t="e" cm="1">
+      <c r="G7" s="143"/>
+      <c r="H7" s="143"/>
+      <c r="I7" s="140" t="e" cm="1">
         <f t="array" aca="1" ref="I7" ca="1">INDIRECT("Sheet1!"&amp;"I9")</f>
         <v>#REF!</v>
       </c>
-      <c r="J7" s="113"/>
-      <c r="K7" s="114"/>
+      <c r="J7" s="140"/>
+      <c r="K7" s="141"/>
     </row>
     <row r="8" spans="1:11" ht="31.5">
-      <c r="A8" s="122" t="s">
+      <c r="A8" s="129" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="107"/>
+      <c r="B8" s="102"/>
       <c r="C8" s="27" t="s">
         <v>10</v>
       </c>
@@ -8019,14 +8058,14 @@
       <c r="E8" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="149" t="s">
+      <c r="F8" s="53" t="s">
         <v>88</v>
       </c>
-      <c r="G8" s="117" t="s">
+      <c r="G8" s="144" t="s">
         <v>13</v>
       </c>
-      <c r="H8" s="106"/>
-      <c r="I8" s="107"/>
+      <c r="H8" s="101"/>
+      <c r="I8" s="102"/>
       <c r="J8" s="27" t="s">
         <v>14</v>
       </c>
@@ -8035,11 +8074,11 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="27.4" customHeight="1">
-      <c r="A9" s="120" t="e" cm="1">
+      <c r="A9" s="130" t="e" cm="1">
         <f t="array" aca="1" ref="A9" ca="1">INDIRECT("Sheet2!"&amp;"E27")</f>
         <v>#REF!</v>
       </c>
-      <c r="B9" s="107"/>
+      <c r="B9" s="102"/>
       <c r="C9" s="29" t="e" cm="1">
         <f t="array" aca="1" ref="C9" ca="1">INDIRECT("Sheet2!"&amp;"A27")</f>
         <v>#REF!</v>
@@ -8053,18 +8092,18 @@
         <v>#REF!</v>
       </c>
       <c r="F9" s="32"/>
-      <c r="G9" s="108"/>
-      <c r="H9" s="106"/>
-      <c r="I9" s="107"/>
+      <c r="G9" s="100"/>
+      <c r="H9" s="101"/>
+      <c r="I9" s="102"/>
       <c r="J9" s="24"/>
       <c r="K9" s="33"/>
     </row>
     <row r="10" spans="1:11" ht="27.4" customHeight="1">
-      <c r="A10" s="118" t="e" cm="1">
+      <c r="A10" s="132" t="e" cm="1">
         <f t="array" aca="1" ref="A10" ca="1">INDIRECT("Sheet2!"&amp;"E28")</f>
         <v>#REF!</v>
       </c>
-      <c r="B10" s="107"/>
+      <c r="B10" s="102"/>
       <c r="C10" s="34" t="e" cm="1">
         <f t="array" aca="1" ref="C10" ca="1">INDIRECT("Sheet2!"&amp;"A28")</f>
         <v>#REF!</v>
@@ -8078,18 +8117,18 @@
         <v>#REF!</v>
       </c>
       <c r="F10" s="37"/>
-      <c r="G10" s="105"/>
-      <c r="H10" s="106"/>
-      <c r="I10" s="107"/>
+      <c r="G10" s="103"/>
+      <c r="H10" s="101"/>
+      <c r="I10" s="102"/>
       <c r="J10" s="38"/>
       <c r="K10" s="39"/>
     </row>
     <row r="11" spans="1:11" ht="27.4" customHeight="1">
-      <c r="A11" s="120" t="e" cm="1">
+      <c r="A11" s="130" t="e" cm="1">
         <f t="array" aca="1" ref="A11" ca="1">INDIRECT("Sheet2!"&amp;"E29")</f>
         <v>#REF!</v>
       </c>
-      <c r="B11" s="107"/>
+      <c r="B11" s="102"/>
       <c r="C11" s="29" t="e" cm="1">
         <f t="array" aca="1" ref="C11" ca="1">INDIRECT("Sheet2!"&amp;"A29")</f>
         <v>#REF!</v>
@@ -8103,18 +8142,18 @@
         <v>#REF!</v>
       </c>
       <c r="F11" s="32"/>
-      <c r="G11" s="108"/>
-      <c r="H11" s="106"/>
-      <c r="I11" s="107"/>
+      <c r="G11" s="100"/>
+      <c r="H11" s="101"/>
+      <c r="I11" s="102"/>
       <c r="J11" s="24"/>
       <c r="K11" s="33"/>
     </row>
     <row r="12" spans="1:11" ht="27.4" customHeight="1">
-      <c r="A12" s="118" t="e" cm="1">
+      <c r="A12" s="132" t="e" cm="1">
         <f t="array" aca="1" ref="A12" ca="1">INDIRECT("Sheet2!"&amp;"E30")</f>
         <v>#REF!</v>
       </c>
-      <c r="B12" s="107"/>
+      <c r="B12" s="102"/>
       <c r="C12" s="40" t="e" cm="1">
         <f t="array" aca="1" ref="C12" ca="1">INDIRECT("Sheet2!"&amp;"A30")</f>
         <v>#REF!</v>
@@ -8128,18 +8167,18 @@
         <v>#REF!</v>
       </c>
       <c r="F12" s="37"/>
-      <c r="G12" s="105"/>
-      <c r="H12" s="106"/>
-      <c r="I12" s="107"/>
+      <c r="G12" s="103"/>
+      <c r="H12" s="101"/>
+      <c r="I12" s="102"/>
       <c r="J12" s="38"/>
       <c r="K12" s="39"/>
     </row>
     <row r="13" spans="1:11" ht="27.4" customHeight="1">
-      <c r="A13" s="120" t="e" cm="1">
+      <c r="A13" s="130" t="e" cm="1">
         <f t="array" aca="1" ref="A13" ca="1">INDIRECT("Sheet2!"&amp;"E31")</f>
         <v>#REF!</v>
       </c>
-      <c r="B13" s="107"/>
+      <c r="B13" s="102"/>
       <c r="C13" s="41" t="e" cm="1">
         <f t="array" aca="1" ref="C13" ca="1">INDIRECT("Sheet2!"&amp;"A31")</f>
         <v>#REF!</v>
@@ -8153,18 +8192,18 @@
         <v>#REF!</v>
       </c>
       <c r="F13" s="32"/>
-      <c r="G13" s="108"/>
-      <c r="H13" s="106"/>
-      <c r="I13" s="107"/>
+      <c r="G13" s="100"/>
+      <c r="H13" s="101"/>
+      <c r="I13" s="102"/>
       <c r="J13" s="24"/>
       <c r="K13" s="33"/>
     </row>
     <row r="14" spans="1:11" ht="27.4" customHeight="1">
-      <c r="A14" s="118" t="e" cm="1">
+      <c r="A14" s="132" t="e" cm="1">
         <f t="array" aca="1" ref="A14" ca="1">INDIRECT("Sheet2!"&amp;"E32")</f>
         <v>#REF!</v>
       </c>
-      <c r="B14" s="107"/>
+      <c r="B14" s="102"/>
       <c r="C14" s="40" t="e" cm="1">
         <f t="array" aca="1" ref="C14" ca="1">INDIRECT("Sheet2!"&amp;"A32")</f>
         <v>#REF!</v>
@@ -8178,18 +8217,18 @@
         <v>#REF!</v>
       </c>
       <c r="F14" s="37"/>
-      <c r="G14" s="105"/>
-      <c r="H14" s="106"/>
-      <c r="I14" s="107"/>
+      <c r="G14" s="103"/>
+      <c r="H14" s="101"/>
+      <c r="I14" s="102"/>
       <c r="J14" s="38"/>
       <c r="K14" s="39"/>
     </row>
     <row r="15" spans="1:11" ht="27.4" customHeight="1">
-      <c r="A15" s="120" t="e" cm="1">
+      <c r="A15" s="130" t="e" cm="1">
         <f t="array" aca="1" ref="A15" ca="1">INDIRECT("Sheet2!"&amp;"E33")</f>
         <v>#REF!</v>
       </c>
-      <c r="B15" s="107"/>
+      <c r="B15" s="102"/>
       <c r="C15" s="41" t="e" cm="1">
         <f t="array" aca="1" ref="C15" ca="1">INDIRECT("Sheet2!"&amp;"A33")</f>
         <v>#REF!</v>
@@ -8203,18 +8242,18 @@
         <v>#REF!</v>
       </c>
       <c r="F15" s="32"/>
-      <c r="G15" s="108"/>
-      <c r="H15" s="106"/>
-      <c r="I15" s="107"/>
+      <c r="G15" s="100"/>
+      <c r="H15" s="101"/>
+      <c r="I15" s="102"/>
       <c r="J15" s="24"/>
       <c r="K15" s="33"/>
     </row>
     <row r="16" spans="1:11" ht="27.4" customHeight="1">
-      <c r="A16" s="118" t="e" cm="1">
+      <c r="A16" s="132" t="e" cm="1">
         <f t="array" aca="1" ref="A16" ca="1">INDIRECT("Sheet2!"&amp;"E34")</f>
         <v>#REF!</v>
       </c>
-      <c r="B16" s="107"/>
+      <c r="B16" s="102"/>
       <c r="C16" s="40" t="e" cm="1">
         <f t="array" aca="1" ref="C16" ca="1">INDIRECT("Sheet2!"&amp;"A34")</f>
         <v>#REF!</v>
@@ -8228,18 +8267,18 @@
         <v>#REF!</v>
       </c>
       <c r="F16" s="37"/>
-      <c r="G16" s="105"/>
-      <c r="H16" s="106"/>
-      <c r="I16" s="107"/>
+      <c r="G16" s="103"/>
+      <c r="H16" s="101"/>
+      <c r="I16" s="102"/>
       <c r="J16" s="38"/>
       <c r="K16" s="39"/>
     </row>
     <row r="17" spans="1:11" ht="27.4" customHeight="1">
-      <c r="A17" s="120" t="e" cm="1">
+      <c r="A17" s="130" t="e" cm="1">
         <f t="array" aca="1" ref="A17" ca="1">INDIRECT("Sheet2!"&amp;"E35")</f>
         <v>#REF!</v>
       </c>
-      <c r="B17" s="107"/>
+      <c r="B17" s="102"/>
       <c r="C17" s="41" t="e" cm="1">
         <f t="array" aca="1" ref="C17" ca="1">INDIRECT("Sheet2!"&amp;"A35")</f>
         <v>#REF!</v>
@@ -8253,18 +8292,18 @@
         <v>#REF!</v>
       </c>
       <c r="F17" s="32"/>
-      <c r="G17" s="108"/>
-      <c r="H17" s="106"/>
-      <c r="I17" s="107"/>
+      <c r="G17" s="100"/>
+      <c r="H17" s="101"/>
+      <c r="I17" s="102"/>
       <c r="J17" s="24"/>
       <c r="K17" s="33"/>
     </row>
     <row r="18" spans="1:11" ht="27.4" customHeight="1">
-      <c r="A18" s="118" t="e" cm="1">
+      <c r="A18" s="132" t="e" cm="1">
         <f t="array" aca="1" ref="A18" ca="1">INDIRECT("Sheet2!"&amp;"E36")</f>
         <v>#REF!</v>
       </c>
-      <c r="B18" s="107"/>
+      <c r="B18" s="102"/>
       <c r="C18" s="40" t="e" cm="1">
         <f t="array" aca="1" ref="C18" ca="1">INDIRECT("Sheet2!"&amp;"A36")</f>
         <v>#REF!</v>
@@ -8278,18 +8317,18 @@
         <v>#REF!</v>
       </c>
       <c r="F18" s="37"/>
-      <c r="G18" s="105"/>
-      <c r="H18" s="106"/>
-      <c r="I18" s="107"/>
+      <c r="G18" s="103"/>
+      <c r="H18" s="101"/>
+      <c r="I18" s="102"/>
       <c r="J18" s="38"/>
       <c r="K18" s="39"/>
     </row>
     <row r="19" spans="1:11" ht="27.4" customHeight="1">
-      <c r="A19" s="120" t="e" cm="1">
+      <c r="A19" s="130" t="e" cm="1">
         <f t="array" aca="1" ref="A19" ca="1">INDIRECT("Sheet2!"&amp;"E37")</f>
         <v>#REF!</v>
       </c>
-      <c r="B19" s="107"/>
+      <c r="B19" s="102"/>
       <c r="C19" s="41" t="e" cm="1">
         <f t="array" aca="1" ref="C19" ca="1">INDIRECT("Sheet2!"&amp;"A37")</f>
         <v>#REF!</v>
@@ -8303,18 +8342,18 @@
         <v>#REF!</v>
       </c>
       <c r="F19" s="32"/>
-      <c r="G19" s="108"/>
-      <c r="H19" s="106"/>
-      <c r="I19" s="107"/>
+      <c r="G19" s="100"/>
+      <c r="H19" s="101"/>
+      <c r="I19" s="102"/>
       <c r="J19" s="24"/>
       <c r="K19" s="33"/>
     </row>
     <row r="20" spans="1:11" ht="27.4" customHeight="1">
-      <c r="A20" s="118" t="e" cm="1">
+      <c r="A20" s="132" t="e" cm="1">
         <f t="array" aca="1" ref="A20" ca="1">INDIRECT("Sheet2!"&amp;"E38")</f>
         <v>#REF!</v>
       </c>
-      <c r="B20" s="107"/>
+      <c r="B20" s="102"/>
       <c r="C20" s="40" t="e" cm="1">
         <f t="array" aca="1" ref="C20" ca="1">INDIRECT("Sheet2!"&amp;"A38")</f>
         <v>#REF!</v>
@@ -8328,18 +8367,18 @@
         <v>#REF!</v>
       </c>
       <c r="F20" s="37"/>
-      <c r="G20" s="105"/>
-      <c r="H20" s="106"/>
-      <c r="I20" s="107"/>
+      <c r="G20" s="103"/>
+      <c r="H20" s="101"/>
+      <c r="I20" s="102"/>
       <c r="J20" s="38"/>
       <c r="K20" s="39"/>
     </row>
     <row r="21" spans="1:11" ht="27.4" customHeight="1">
-      <c r="A21" s="120" t="e" cm="1">
+      <c r="A21" s="130" t="e" cm="1">
         <f t="array" aca="1" ref="A21" ca="1">INDIRECT("Sheet2!"&amp;"E39")</f>
         <v>#REF!</v>
       </c>
-      <c r="B21" s="107"/>
+      <c r="B21" s="102"/>
       <c r="C21" s="41" t="e" cm="1">
         <f t="array" aca="1" ref="C21" ca="1">INDIRECT("Sheet2!"&amp;"A39")</f>
         <v>#REF!</v>
@@ -8353,18 +8392,18 @@
         <v>#REF!</v>
       </c>
       <c r="F21" s="32"/>
-      <c r="G21" s="108"/>
-      <c r="H21" s="106"/>
-      <c r="I21" s="107"/>
+      <c r="G21" s="100"/>
+      <c r="H21" s="101"/>
+      <c r="I21" s="102"/>
       <c r="J21" s="24"/>
       <c r="K21" s="33"/>
     </row>
     <row r="22" spans="1:11" ht="27.4" customHeight="1">
-      <c r="A22" s="118" t="e" cm="1">
+      <c r="A22" s="132" t="e" cm="1">
         <f t="array" aca="1" ref="A22" ca="1">INDIRECT("Sheet2!"&amp;"E40")</f>
         <v>#REF!</v>
       </c>
-      <c r="B22" s="107"/>
+      <c r="B22" s="102"/>
       <c r="C22" s="40" t="e" cm="1">
         <f t="array" aca="1" ref="C22" ca="1">INDIRECT("Sheet2!"&amp;"A40")</f>
         <v>#REF!</v>
@@ -8378,18 +8417,18 @@
         <v>#REF!</v>
       </c>
       <c r="F22" s="37"/>
-      <c r="G22" s="105"/>
-      <c r="H22" s="106"/>
-      <c r="I22" s="107"/>
+      <c r="G22" s="103"/>
+      <c r="H22" s="101"/>
+      <c r="I22" s="102"/>
       <c r="J22" s="38"/>
       <c r="K22" s="39"/>
     </row>
     <row r="23" spans="1:11" ht="27.4" customHeight="1">
-      <c r="A23" s="120" t="e" cm="1">
+      <c r="A23" s="130" t="e" cm="1">
         <f t="array" aca="1" ref="A23" ca="1">INDIRECT("Sheet2!"&amp;"E41")</f>
         <v>#REF!</v>
       </c>
-      <c r="B23" s="107"/>
+      <c r="B23" s="102"/>
       <c r="C23" s="41" t="e" cm="1">
         <f t="array" aca="1" ref="C23" ca="1">INDIRECT("Sheet2!"&amp;"A41")</f>
         <v>#REF!</v>
@@ -8403,18 +8442,18 @@
         <v>#REF!</v>
       </c>
       <c r="F23" s="32"/>
-      <c r="G23" s="108"/>
-      <c r="H23" s="106"/>
-      <c r="I23" s="107"/>
+      <c r="G23" s="100"/>
+      <c r="H23" s="101"/>
+      <c r="I23" s="102"/>
       <c r="J23" s="24"/>
       <c r="K23" s="33"/>
     </row>
     <row r="24" spans="1:11" ht="27.4" customHeight="1">
-      <c r="A24" s="118" t="e" cm="1">
+      <c r="A24" s="132" t="e" cm="1">
         <f t="array" aca="1" ref="A24" ca="1">INDIRECT("Sheet2!"&amp;"E42")</f>
         <v>#REF!</v>
       </c>
-      <c r="B24" s="107"/>
+      <c r="B24" s="102"/>
       <c r="C24" s="40" t="e" cm="1">
         <f t="array" aca="1" ref="C24" ca="1">INDIRECT("Sheet2!"&amp;"A42")</f>
         <v>#REF!</v>
@@ -8428,18 +8467,18 @@
         <v>#REF!</v>
       </c>
       <c r="F24" s="37"/>
-      <c r="G24" s="105"/>
-      <c r="H24" s="106"/>
-      <c r="I24" s="107"/>
+      <c r="G24" s="103"/>
+      <c r="H24" s="101"/>
+      <c r="I24" s="102"/>
       <c r="J24" s="38"/>
       <c r="K24" s="39"/>
     </row>
     <row r="25" spans="1:11" ht="27.4" customHeight="1">
-      <c r="A25" s="120" t="e" cm="1">
+      <c r="A25" s="130" t="e" cm="1">
         <f t="array" aca="1" ref="A25" ca="1">INDIRECT("Sheet2!"&amp;"E43")</f>
         <v>#REF!</v>
       </c>
-      <c r="B25" s="107"/>
+      <c r="B25" s="102"/>
       <c r="C25" s="41" t="e" cm="1">
         <f t="array" aca="1" ref="C25" ca="1">INDIRECT("Sheet2!"&amp;"A43")</f>
         <v>#REF!</v>
@@ -8453,18 +8492,18 @@
         <v>#REF!</v>
       </c>
       <c r="F25" s="32"/>
-      <c r="G25" s="108"/>
-      <c r="H25" s="106"/>
-      <c r="I25" s="107"/>
+      <c r="G25" s="100"/>
+      <c r="H25" s="101"/>
+      <c r="I25" s="102"/>
       <c r="J25" s="24"/>
       <c r="K25" s="33"/>
     </row>
     <row r="26" spans="1:11" ht="27.4" customHeight="1">
-      <c r="A26" s="118" t="e" cm="1">
+      <c r="A26" s="132" t="e" cm="1">
         <f t="array" aca="1" ref="A26" ca="1">INDIRECT("Sheet2!"&amp;"E44")</f>
         <v>#REF!</v>
       </c>
-      <c r="B26" s="107"/>
+      <c r="B26" s="102"/>
       <c r="C26" s="40" t="e" cm="1">
         <f t="array" aca="1" ref="C26" ca="1">INDIRECT("Sheet2!"&amp;"A44")</f>
         <v>#REF!</v>
@@ -8478,177 +8517,177 @@
         <v>#REF!</v>
       </c>
       <c r="F26" s="37"/>
-      <c r="G26" s="105"/>
-      <c r="H26" s="106"/>
-      <c r="I26" s="107"/>
+      <c r="G26" s="103"/>
+      <c r="H26" s="101"/>
+      <c r="I26" s="102"/>
       <c r="J26" s="38"/>
       <c r="K26" s="39"/>
     </row>
     <row r="27" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A27" s="146" t="s">
+      <c r="A27" s="104" t="s">
         <v>16</v>
       </c>
-      <c r="B27" s="124"/>
-      <c r="C27" s="124"/>
-      <c r="D27" s="124"/>
-      <c r="E27" s="124"/>
-      <c r="F27" s="124"/>
-      <c r="G27" s="124"/>
-      <c r="H27" s="125"/>
+      <c r="B27" s="105"/>
+      <c r="C27" s="105"/>
+      <c r="D27" s="105"/>
+      <c r="E27" s="105"/>
+      <c r="F27" s="105"/>
+      <c r="G27" s="105"/>
+      <c r="H27" s="106"/>
       <c r="I27" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="J27" s="144" t="s">
+      <c r="J27" s="109" t="s">
         <v>18</v>
       </c>
-      <c r="K27" s="145"/>
+      <c r="K27" s="110"/>
     </row>
     <row r="28" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A28" s="141" t="s">
+      <c r="A28" s="113" t="s">
         <v>19</v>
       </c>
-      <c r="B28" s="106"/>
-      <c r="C28" s="106"/>
-      <c r="D28" s="106"/>
-      <c r="E28" s="106"/>
-      <c r="F28" s="106"/>
-      <c r="G28" s="106"/>
-      <c r="H28" s="107"/>
+      <c r="B28" s="101"/>
+      <c r="C28" s="101"/>
+      <c r="D28" s="101"/>
+      <c r="E28" s="101"/>
+      <c r="F28" s="101"/>
+      <c r="G28" s="101"/>
+      <c r="H28" s="102"/>
       <c r="I28" s="43"/>
-      <c r="J28" s="142"/>
-      <c r="K28" s="143"/>
+      <c r="J28" s="111"/>
+      <c r="K28" s="112"/>
     </row>
     <row r="29" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A29" s="141" t="s">
+      <c r="A29" s="113" t="s">
         <v>20</v>
       </c>
-      <c r="B29" s="106"/>
-      <c r="C29" s="106"/>
-      <c r="D29" s="106"/>
-      <c r="E29" s="106"/>
-      <c r="F29" s="106"/>
-      <c r="G29" s="106"/>
-      <c r="H29" s="107"/>
+      <c r="B29" s="101"/>
+      <c r="C29" s="101"/>
+      <c r="D29" s="101"/>
+      <c r="E29" s="101"/>
+      <c r="F29" s="101"/>
+      <c r="G29" s="101"/>
+      <c r="H29" s="102"/>
       <c r="I29" s="43"/>
-      <c r="J29" s="142"/>
-      <c r="K29" s="143"/>
+      <c r="J29" s="111"/>
+      <c r="K29" s="112"/>
     </row>
     <row r="30" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A30" s="141" t="s">
+      <c r="A30" s="113" t="s">
         <v>21</v>
       </c>
-      <c r="B30" s="106"/>
-      <c r="C30" s="106"/>
-      <c r="D30" s="106"/>
-      <c r="E30" s="106"/>
-      <c r="F30" s="106"/>
-      <c r="G30" s="106"/>
-      <c r="H30" s="107"/>
+      <c r="B30" s="101"/>
+      <c r="C30" s="101"/>
+      <c r="D30" s="101"/>
+      <c r="E30" s="101"/>
+      <c r="F30" s="101"/>
+      <c r="G30" s="101"/>
+      <c r="H30" s="102"/>
       <c r="I30" s="43"/>
-      <c r="J30" s="142"/>
-      <c r="K30" s="143"/>
+      <c r="J30" s="111"/>
+      <c r="K30" s="112"/>
     </row>
     <row r="31" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A31" s="141" t="s">
+      <c r="A31" s="113" t="s">
         <v>22</v>
       </c>
-      <c r="B31" s="106"/>
-      <c r="C31" s="106"/>
-      <c r="D31" s="106"/>
-      <c r="E31" s="106"/>
-      <c r="F31" s="106"/>
-      <c r="G31" s="106"/>
-      <c r="H31" s="107"/>
+      <c r="B31" s="101"/>
+      <c r="C31" s="101"/>
+      <c r="D31" s="101"/>
+      <c r="E31" s="101"/>
+      <c r="F31" s="101"/>
+      <c r="G31" s="101"/>
+      <c r="H31" s="102"/>
       <c r="I31" s="43"/>
-      <c r="J31" s="142"/>
-      <c r="K31" s="143"/>
+      <c r="J31" s="111"/>
+      <c r="K31" s="112"/>
     </row>
     <row r="32" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A32" s="141" t="s">
+      <c r="A32" s="113" t="s">
         <v>23</v>
       </c>
-      <c r="B32" s="106"/>
-      <c r="C32" s="106"/>
-      <c r="D32" s="106"/>
-      <c r="E32" s="106"/>
-      <c r="F32" s="106"/>
-      <c r="G32" s="106"/>
-      <c r="H32" s="107"/>
+      <c r="B32" s="101"/>
+      <c r="C32" s="101"/>
+      <c r="D32" s="101"/>
+      <c r="E32" s="101"/>
+      <c r="F32" s="101"/>
+      <c r="G32" s="101"/>
+      <c r="H32" s="102"/>
       <c r="I32" s="43"/>
-      <c r="J32" s="142"/>
-      <c r="K32" s="143"/>
+      <c r="J32" s="111"/>
+      <c r="K32" s="112"/>
     </row>
     <row r="33" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A33" s="141" t="s">
+      <c r="A33" s="113" t="s">
         <v>24</v>
       </c>
-      <c r="B33" s="106"/>
-      <c r="C33" s="106"/>
-      <c r="D33" s="106"/>
-      <c r="E33" s="106"/>
-      <c r="F33" s="106"/>
-      <c r="G33" s="106"/>
-      <c r="H33" s="107"/>
+      <c r="B33" s="101"/>
+      <c r="C33" s="101"/>
+      <c r="D33" s="101"/>
+      <c r="E33" s="101"/>
+      <c r="F33" s="101"/>
+      <c r="G33" s="101"/>
+      <c r="H33" s="102"/>
       <c r="I33" s="43"/>
-      <c r="J33" s="142"/>
-      <c r="K33" s="143"/>
+      <c r="J33" s="111"/>
+      <c r="K33" s="112"/>
     </row>
     <row r="34" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A34" s="141" t="s">
+      <c r="A34" s="113" t="s">
         <v>25</v>
       </c>
-      <c r="B34" s="106"/>
-      <c r="C34" s="106"/>
-      <c r="D34" s="106"/>
-      <c r="E34" s="106"/>
-      <c r="F34" s="106"/>
-      <c r="G34" s="106"/>
-      <c r="H34" s="107"/>
+      <c r="B34" s="101"/>
+      <c r="C34" s="101"/>
+      <c r="D34" s="101"/>
+      <c r="E34" s="101"/>
+      <c r="F34" s="101"/>
+      <c r="G34" s="101"/>
+      <c r="H34" s="102"/>
       <c r="I34" s="43"/>
-      <c r="J34" s="142"/>
-      <c r="K34" s="143"/>
+      <c r="J34" s="111"/>
+      <c r="K34" s="112"/>
     </row>
     <row r="35" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A35" s="100" t="s">
+      <c r="A35" s="146" t="s">
         <v>79</v>
       </c>
-      <c r="B35" s="101"/>
-      <c r="C35" s="101"/>
-      <c r="D35" s="101"/>
-      <c r="E35" s="101"/>
-      <c r="F35" s="101"/>
-      <c r="G35" s="101"/>
-      <c r="H35" s="102"/>
+      <c r="B35" s="147"/>
+      <c r="C35" s="147"/>
+      <c r="D35" s="147"/>
+      <c r="E35" s="147"/>
+      <c r="F35" s="147"/>
+      <c r="G35" s="147"/>
+      <c r="H35" s="148"/>
       <c r="I35" s="47"/>
-      <c r="J35" s="103"/>
-      <c r="K35" s="104"/>
+      <c r="J35" s="149"/>
+      <c r="K35" s="126"/>
     </row>
     <row r="36" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A36" s="99" t="s">
+      <c r="A36" s="145" t="s">
         <v>80</v>
       </c>
-      <c r="B36" s="99"/>
+      <c r="B36" s="145"/>
       <c r="C36" s="48"/>
     </row>
     <row r="37" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A37" s="99" t="s">
+      <c r="A37" s="145" t="s">
         <v>82</v>
       </c>
-      <c r="B37" s="99"/>
+      <c r="B37" s="145"/>
       <c r="C37" s="48"/>
     </row>
     <row r="38" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A38" s="99" t="s">
+      <c r="A38" s="145" t="s">
         <v>81</v>
       </c>
-      <c r="B38" s="99"/>
+      <c r="B38" s="145"/>
       <c r="C38" s="48"/>
     </row>
     <row r="39" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A39" s="99" t="s">
+      <c r="A39" s="145" t="s">
         <v>83</v>
       </c>
-      <c r="B39" s="99"/>
+      <c r="B39" s="145"/>
       <c r="C39" s="48"/>
     </row>
     <row r="40" spans="1:11" ht="15.75" customHeight="1"/>
@@ -9614,60 +9653,12 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="73">
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="G24:I24"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="G26:I26"/>
-    <mergeCell ref="A27:H27"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="J31:K31"/>
-    <mergeCell ref="J32:K32"/>
-    <mergeCell ref="A33:H33"/>
-    <mergeCell ref="J33:K33"/>
-    <mergeCell ref="A34:H34"/>
-    <mergeCell ref="J34:K34"/>
-    <mergeCell ref="A28:H28"/>
-    <mergeCell ref="A29:H29"/>
-    <mergeCell ref="J29:K29"/>
-    <mergeCell ref="A30:H30"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="A31:H31"/>
-    <mergeCell ref="A32:H32"/>
-    <mergeCell ref="A1:B5"/>
-    <mergeCell ref="C1:H5"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="G9:I9"/>
-    <mergeCell ref="G10:I10"/>
-    <mergeCell ref="G11:I11"/>
-    <mergeCell ref="G12:I12"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="G14:I14"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A35:H35"/>
+    <mergeCell ref="J35:K35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A38:B38"/>
     <mergeCell ref="G20:I20"/>
     <mergeCell ref="G21:I21"/>
     <mergeCell ref="G22:I22"/>
@@ -9681,12 +9672,60 @@
     <mergeCell ref="G18:I18"/>
     <mergeCell ref="G19:I19"/>
     <mergeCell ref="G8:I8"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A35:H35"/>
-    <mergeCell ref="J35:K35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="G10:I10"/>
+    <mergeCell ref="G11:I11"/>
+    <mergeCell ref="G12:I12"/>
+    <mergeCell ref="G13:I13"/>
+    <mergeCell ref="G14:I14"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="A1:B5"/>
+    <mergeCell ref="C1:H5"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="A34:H34"/>
+    <mergeCell ref="J34:K34"/>
+    <mergeCell ref="A28:H28"/>
+    <mergeCell ref="A29:H29"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="A30:H30"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="A31:H31"/>
+    <mergeCell ref="A32:H32"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="J31:K31"/>
+    <mergeCell ref="J32:K32"/>
+    <mergeCell ref="A33:H33"/>
+    <mergeCell ref="J33:K33"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="A27:H27"/>
+    <mergeCell ref="A26:B26"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.33" bottom="0.28000000000000003" header="0" footer="0"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="landscape"/>

</xml_diff>